<commit_message>
final video and upgraded audio
</commit_message>
<xml_diff>
--- a/Crawler/App_direct_links.xlsx
+++ b/Crawler/App_direct_links.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Desktop\Final_Project\Crawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C12322-725B-4998-B302-F023D0C0E81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC31D83-D17E-40CC-A59C-B2756C5BAC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12780" yWindow="3885" windowWidth="12810" windowHeight="12000" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FINAL" sheetId="16" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="1505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="1508">
   <si>
     <t>Khan Academy</t>
   </si>
@@ -3914,9 +3914,6 @@
     <t>app-btn-primary</t>
   </si>
   <si>
-    <t>css-19qwy7b</t>
-  </si>
-  <si>
     <t>קישור</t>
   </si>
   <si>
@@ -3959,15 +3956,9 @@
     <t>ud-custom-focus-visible</t>
   </si>
   <si>
-    <t>sp_choice_type_11</t>
-  </si>
-  <si>
     <t>didomi-notice-agree-button</t>
   </si>
   <si>
-    <t>cmptxt_btn_yes</t>
-  </si>
-  <si>
     <t>PlayButton-base</t>
   </si>
   <si>
@@ -4560,6 +4551,24 @@
   </si>
   <si>
     <t>https://holla.world</t>
+  </si>
+  <si>
+    <t>wobbly-bouncy</t>
+  </si>
+  <si>
+    <t>https://www.nick.co.il/brand/4</t>
+  </si>
+  <si>
+    <t>popup__close</t>
+  </si>
+  <si>
+    <t>https://www.pbs.org/newshour/show/what-to-know-about-the-start-of-negotiations-between-iran-and-the-u-s-under-trump</t>
+  </si>
+  <si>
+    <t>gdpr-btn-accept-all,css-19qwy7b</t>
+  </si>
+  <si>
+    <t>https://www.retrocrush.tv/watch/1000000012595/title1?vod_type=</t>
   </si>
 </sst>
 </file>
@@ -9614,13 +9623,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C1" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -10132,515 +10141,516 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B00D6D-F8EE-49C3-8560-55C57AAB910F}">
   <dimension ref="C2:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
-        <v>1313</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="3" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
-        <v>1314</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
-        <v>1315</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
-        <v>1316</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
-        <v>1317</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
-        <v>1318</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="9" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
-        <v>1320</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="10" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="11" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="12" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
-        <v>1323</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="13" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
-        <v>1324</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="14" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
-        <v>1325</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="15" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
-        <v>1326</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="16" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
-        <v>1327</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
-        <v>1328</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
-        <v>1329</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
-        <v>1330</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
-        <v>1331</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
-        <v>1332</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
-        <v>1333</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
-        <v>1334</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
-        <v>1335</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
-        <v>1336</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
-        <v>1337</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
-        <v>1338</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" s="3" t="s">
-        <v>1339</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="s">
-        <v>1341</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31" s="3" t="s">
-        <v>1342</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32" s="3" t="s">
-        <v>1343</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
-        <v>1344</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="3" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="3" t="s">
-        <v>1347</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="3" t="s">
-        <v>1348</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="3" t="s">
-        <v>1349</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="3" t="s">
-        <v>1350</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="3" t="s">
-        <v>1351</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="3" t="s">
-        <v>1352</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="3" t="s">
-        <v>1353</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="3" t="s">
-        <v>1354</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" s="3" t="s">
-        <v>1355</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="3" t="s">
-        <v>1356</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" s="3" t="s">
-        <v>1357</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="3" t="s">
-        <v>1358</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="3" t="s">
-        <v>1359</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="3" t="s">
-        <v>1360</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="3" t="s">
-        <v>1361</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="3" t="s">
-        <v>1362</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="3" t="s">
-        <v>1363</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="3" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="3" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="3" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="3" t="s">
-        <v>1367</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="3" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="3" t="s">
-        <v>1369</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="3" t="s">
-        <v>1370</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="3" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="3" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="3" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="3" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" s="3" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" s="3" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" s="3" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="3" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" s="3" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" s="3" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" s="3" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" s="3" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" s="3" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" s="3" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" s="3" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" s="3" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" s="3" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="3" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" s="3" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" s="3" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" s="3" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="3" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" s="3" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="3" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" s="3" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="3" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86" s="3" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="3" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C88" s="3" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" s="3" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C90" s="3" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="3" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" s="3" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="3" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C94" s="3" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="3" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" s="3" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="3" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" s="3" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="3" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" s="3" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="3" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{646957ED-0A75-459A-99B7-3F1A0DCFE246}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{51AF03CB-8730-4798-8C6C-9AD72FFC79D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10658,7 +10668,7 @@
   <sheetData>
     <row r="2" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="3" spans="3:3" x14ac:dyDescent="0.25">
@@ -10668,42 +10678,42 @@
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
-        <v>1414</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
-        <v>1415</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="9" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="10" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="11" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="12" spans="3:3" x14ac:dyDescent="0.25">
@@ -10718,7 +10728,7 @@
     </row>
     <row r="14" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="15" spans="3:3" x14ac:dyDescent="0.25">
@@ -10728,12 +10738,12 @@
     </row>
     <row r="16" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C16" s="5" t="s">
-        <v>1423</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="5" t="s">
-        <v>1424</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
@@ -10743,417 +10753,417 @@
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="5" t="s">
-        <v>1425</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="5" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="5" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="5" t="s">
-        <v>1428</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="5" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" s="5" t="s">
-        <v>1430</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" s="5" t="s">
-        <v>1431</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" s="5" t="s">
-        <v>1432</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" s="5" t="s">
-        <v>1433</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" s="5" t="s">
-        <v>1434</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" s="5" t="s">
-        <v>1435</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30" s="5" t="s">
-        <v>1436</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31" s="5" t="s">
-        <v>1437</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32" s="5" t="s">
-        <v>1438</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="5" t="s">
-        <v>1439</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="5" t="s">
-        <v>1440</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
-        <v>1441</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="5" t="s">
-        <v>1442</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="5" t="s">
-        <v>1443</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="5" t="s">
-        <v>1444</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="5" t="s">
-        <v>1445</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="5" t="s">
-        <v>1446</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="5" t="s">
-        <v>1447</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="5" t="s">
-        <v>1448</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="5" t="s">
-        <v>1449</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" s="5" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="5" t="s">
-        <v>1451</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" s="5" t="s">
-        <v>1452</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="5" t="s">
-        <v>1453</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="5" t="s">
-        <v>1454</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="5" t="s">
-        <v>1455</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="5" t="s">
-        <v>1456</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="5" t="s">
-        <v>1457</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="5" t="s">
-        <v>1458</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="5" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="5" t="s">
-        <v>1460</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="5" t="s">
-        <v>1461</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="5" t="s">
-        <v>1462</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="5" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="5" t="s">
-        <v>1464</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="5" t="s">
-        <v>1465</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="5" t="s">
-        <v>1466</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="5" t="s">
-        <v>1467</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="5" t="s">
-        <v>1468</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="5" t="s">
-        <v>1469</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" s="5" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" s="5" t="s">
-        <v>1471</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" s="5" t="s">
-        <v>1472</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="5" t="s">
-        <v>1473</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" s="5" t="s">
-        <v>1474</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" s="5" t="s">
-        <v>1475</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" s="5" t="s">
-        <v>1476</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" s="5" t="s">
-        <v>1477</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" s="5" t="s">
-        <v>1478</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" s="5" t="s">
-        <v>1479</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" s="5" t="s">
-        <v>1480</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" s="5" t="s">
-        <v>1481</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" s="5" t="s">
-        <v>1482</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="5" t="s">
-        <v>1483</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" s="5" t="s">
-        <v>1484</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" s="5" t="s">
-        <v>1485</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" s="5" t="s">
-        <v>1486</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="5" t="s">
-        <v>1487</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" s="5" t="s">
-        <v>1488</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="5" t="s">
-        <v>1489</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" s="5" t="s">
-        <v>1490</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="5" t="s">
-        <v>1491</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86" s="5" t="s">
-        <v>1492</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="5" t="s">
-        <v>1493</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C88" s="5" t="s">
-        <v>1494</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" s="5" t="s">
-        <v>1495</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C90" s="5" t="s">
-        <v>1496</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="5" t="s">
-        <v>1497</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" s="5" t="s">
-        <v>1498</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="5" t="s">
-        <v>1499</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C94" s="5" t="s">
-        <v>1500</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="5" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" s="5" t="s">
-        <v>1434</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="5" t="s">
-        <v>1501</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" s="5" t="s">
-        <v>1502</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="5" t="s">
-        <v>1503</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" s="5" t="s">
-        <v>1504</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" s="5" t="s">
-        <v>1451</v>
+        <v>1448</v>
       </c>
     </row>
   </sheetData>
@@ -11165,8 +11175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F866F9-5AE4-4932-ABC3-52361087BB04}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11178,13 +11188,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C1" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -11226,7 +11236,7 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
       <c r="C8" s="3" t="s">
-        <v>855</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -11307,7 +11317,7 @@
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="15" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>971</v>
@@ -11315,7 +11325,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>884</v>
@@ -11337,7 +11347,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>886</v>
@@ -11345,7 +11355,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>873</v>
@@ -11357,9 +11367,11 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="15"/>
+      <c r="B28" s="19" t="s">
+        <v>1504</v>
+      </c>
       <c r="C28" s="3" t="s">
-        <v>875</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -11377,7 +11389,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="19" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>881</v>
@@ -11406,10 +11418,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>897</v>
@@ -11417,7 +11429,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="19" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>898</v>
@@ -11425,7 +11437,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" s="19" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>899</v>
@@ -11438,7 +11450,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" s="19" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>901</v>
@@ -11455,283 +11467,281 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>1304</v>
+      <c r="B43" s="19" t="s">
+        <v>1303</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="19" t="s">
-        <v>1305</v>
-      </c>
+      <c r="B44" s="19"/>
       <c r="C44" s="3" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="19" t="s">
-        <v>1306</v>
-      </c>
       <c r="C45" s="3" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C46" s="3" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="19" t="s">
+        <v>1304</v>
+      </c>
       <c r="C47" s="3" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="19" t="s">
+      <c r="C48" s="3" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="19" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="3" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="19" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="19"/>
+      <c r="C52" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="19" t="s">
         <v>1307</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C49" s="3" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="19" t="s">
+      <c r="C53" s="3" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="3" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="19" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>1308</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C51" s="3" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="19" t="s">
-        <v>1309</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="19"/>
-      <c r="C53" s="3" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="19" t="s">
-        <v>1310</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C55" s="3" t="s">
-        <v>927</v>
-      </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="19" t="s">
-        <v>1312</v>
-      </c>
       <c r="C56" s="4" t="s">
-        <v>1311</v>
+        <v>930</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C57" s="4" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C58" s="4" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C59" s="4" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C60" s="4" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C61" s="4" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C62" s="4" t="s">
-        <v>937</v>
+      <c r="C62" s="14" t="s">
+        <v>942</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C63" s="14" t="s">
-        <v>942</v>
+      <c r="C63" t="s">
+        <v>945</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C66" s="4" t="s">
-        <v>1297</v>
-      </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="21" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="11" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C67" s="11" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C68" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C69" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C70" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C71" s="11" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C72" s="11" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C73" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C74" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C75" s="11" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C76" s="11" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C77" s="11" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C78" s="11" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C79" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C80" s="11" t="s">
-        <v>577</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C81" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C82" s="11" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C83" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C84" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C85" s="11" t="s">
-        <v>6</v>
+        <v>581</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C86" s="11" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C87" s="11" t="s">
-        <v>582</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C88" s="11" t="s">
-        <v>8</v>
+        <v>583</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C89" s="11" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C90" s="11" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C91" s="11" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C92" s="11" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C93" s="11" t="s">
-        <v>580</v>
+      <c r="C93" s="23" t="s">
+        <v>1296</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
@@ -11781,33 +11791,33 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{8864BEEE-0484-418C-ADFA-89FED57056F0}"/>
     <hyperlink ref="C6" r:id="rId2" xr:uid="{33C07D58-FC14-4694-85DC-CA3F19D77A58}"/>
-    <hyperlink ref="C67" r:id="rId3" display="http://slither.io/" xr:uid="{5D8BF003-D30B-4778-8D41-ABA23E2DC48F}"/>
-    <hyperlink ref="C68" r:id="rId4" display="http://agar.io/" xr:uid="{EDEF75C6-62A1-45D1-A370-18C9E9E7A5EB}"/>
-    <hyperlink ref="C69" r:id="rId5" display="http://diep.io/" xr:uid="{C081F28C-85D7-4926-91CC-DA9AFCFAC301}"/>
-    <hyperlink ref="C70" r:id="rId6" display="http://krunker.io/" xr:uid="{4F654821-B6BF-414A-9C5D-E4E686E2FDCC}"/>
-    <hyperlink ref="C71" r:id="rId7" display="http://skribbl.io/" xr:uid="{E3DE4095-95AF-4E16-A3E9-26D48ABA897C}"/>
-    <hyperlink ref="C72" r:id="rId8" display="http://wings.io/" xr:uid="{FA51F25D-573A-478E-915F-539382CD794B}"/>
-    <hyperlink ref="C73" r:id="rId9" display="http://hole.io/" xr:uid="{3412DE3F-6F60-41D6-9FD5-82534A155FD5}"/>
-    <hyperlink ref="C74" r:id="rId10" display="http://paper.io/" xr:uid="{8010C012-9084-4C91-8B11-7B745C69D5AB}"/>
-    <hyperlink ref="C75" r:id="rId11" display="http://shellshock.io/" xr:uid="{2AD557BC-56C1-450D-8852-CF03B6A65637}"/>
-    <hyperlink ref="C76" r:id="rId12" display="http://snake.io/" xr:uid="{B3934B02-5565-4192-BF7E-1797200AB1C8}"/>
-    <hyperlink ref="C77" r:id="rId13" display="https://www.crazygames.com/game/agario" xr:uid="{3CCD6A56-8988-4C0C-BC37-DB5B15C98F15}"/>
-    <hyperlink ref="C78" r:id="rId14" display="https://www.crazygames.com/game/holey-io-battle-royale" xr:uid="{6144F034-DF98-4F8C-9993-043FB24B3AEF}"/>
-    <hyperlink ref="C79" r:id="rId15" display="https://www.crazygames.com/game/snake-io" xr:uid="{D19B0FEA-6A3B-4B6C-819A-958AE9EE4B92}"/>
-    <hyperlink ref="C80" r:id="rId16" display="https://www.crazygames.com/game/worm-hunt" xr:uid="{E6A299D4-9C16-4E25-BB16-AE333685FBD9}"/>
-    <hyperlink ref="C81" r:id="rId17" display="https://www.crazygames.com/game/paper-io-2" xr:uid="{221E2F90-49CD-4110-9813-9FA920C543E6}"/>
-    <hyperlink ref="C82" r:id="rId18" display="https://www.crazygames.com/game/shellshockersio" xr:uid="{D974E627-1AAF-42B5-876A-FF9DF261A6A3}"/>
-    <hyperlink ref="C83" r:id="rId19" display="https://www.crazygames.com/game/krunker-io" xr:uid="{51942A3B-7EFC-4C4B-BEE1-7E3470295EA2}"/>
-    <hyperlink ref="C90" r:id="rId20" display="https://www.crazygames.com/game/deadshot-io" xr:uid="{5A03ABEE-6E3A-4526-9F2B-73F0AB9B18BB}"/>
-    <hyperlink ref="C92" r:id="rId21" display="https://www.crazygames.com/game/1v1-lol" xr:uid="{A0BA408D-D347-4BA0-9B94-3BE0B489F493}"/>
-    <hyperlink ref="C93" r:id="rId22" display="https://www.crazygames.com/game/diepio" xr:uid="{B2261812-D809-44FA-A72F-AF1D15359AD4}"/>
-    <hyperlink ref="C85" r:id="rId23" display="https://www.crazygames.com/game/buildroyale-io" xr:uid="{ED0498AB-688F-4EE5-BA70-A6D70EBE3684}"/>
-    <hyperlink ref="C86" r:id="rId24" display="https://www.crazygames.com/game/flyordieio" xr:uid="{382FB2BD-8DEF-405F-BE05-B619F1BB4D1D}"/>
-    <hyperlink ref="C87" r:id="rId25" display="https://www.crazygames.com/game/ducklings" xr:uid="{2424889D-FC6A-4203-AE6A-0D896370241B}"/>
-    <hyperlink ref="C88" r:id="rId26" display="https://www.crazygames.com/game/smash-karts" xr:uid="{CB73B8E1-AECC-4B35-A1AA-5FF59EAF37B2}"/>
-    <hyperlink ref="C89" r:id="rId27" display="https://www.crazygames.com/game/bloxdhop-io" xr:uid="{9BC3A4E9-E8DE-402B-9705-3C34244CCBCD}"/>
-    <hyperlink ref="C91" r:id="rId28" display="https://www.crazygames.com/game/skribblio" xr:uid="{1D9AC806-94C6-44C6-A62E-358D25E6CF23}"/>
-    <hyperlink ref="C84" r:id="rId29" display="https://www.crazygames.com/game/taming-io" xr:uid="{6BAB78B7-B303-4AF1-8CDA-B9A0E30451E2}"/>
+    <hyperlink ref="C66" r:id="rId3" display="http://slither.io/" xr:uid="{5D8BF003-D30B-4778-8D41-ABA23E2DC48F}"/>
+    <hyperlink ref="C67" r:id="rId4" display="http://agar.io/" xr:uid="{EDEF75C6-62A1-45D1-A370-18C9E9E7A5EB}"/>
+    <hyperlink ref="C68" r:id="rId5" display="http://diep.io/" xr:uid="{C081F28C-85D7-4926-91CC-DA9AFCFAC301}"/>
+    <hyperlink ref="C69" r:id="rId6" display="http://krunker.io/" xr:uid="{4F654821-B6BF-414A-9C5D-E4E686E2FDCC}"/>
+    <hyperlink ref="C70" r:id="rId7" display="http://skribbl.io/" xr:uid="{E3DE4095-95AF-4E16-A3E9-26D48ABA897C}"/>
+    <hyperlink ref="C71" r:id="rId8" display="http://wings.io/" xr:uid="{FA51F25D-573A-478E-915F-539382CD794B}"/>
+    <hyperlink ref="C72" r:id="rId9" display="http://hole.io/" xr:uid="{3412DE3F-6F60-41D6-9FD5-82534A155FD5}"/>
+    <hyperlink ref="C73" r:id="rId10" display="http://paper.io/" xr:uid="{8010C012-9084-4C91-8B11-7B745C69D5AB}"/>
+    <hyperlink ref="C74" r:id="rId11" display="http://shellshock.io/" xr:uid="{2AD557BC-56C1-450D-8852-CF03B6A65637}"/>
+    <hyperlink ref="C75" r:id="rId12" display="http://snake.io/" xr:uid="{B3934B02-5565-4192-BF7E-1797200AB1C8}"/>
+    <hyperlink ref="C76" r:id="rId13" display="https://www.crazygames.com/game/agario" xr:uid="{3CCD6A56-8988-4C0C-BC37-DB5B15C98F15}"/>
+    <hyperlink ref="C77" r:id="rId14" display="https://www.crazygames.com/game/holey-io-battle-royale" xr:uid="{6144F034-DF98-4F8C-9993-043FB24B3AEF}"/>
+    <hyperlink ref="C78" r:id="rId15" display="https://www.crazygames.com/game/snake-io" xr:uid="{D19B0FEA-6A3B-4B6C-819A-958AE9EE4B92}"/>
+    <hyperlink ref="C79" r:id="rId16" display="https://www.crazygames.com/game/worm-hunt" xr:uid="{E6A299D4-9C16-4E25-BB16-AE333685FBD9}"/>
+    <hyperlink ref="C80" r:id="rId17" display="https://www.crazygames.com/game/paper-io-2" xr:uid="{221E2F90-49CD-4110-9813-9FA920C543E6}"/>
+    <hyperlink ref="C81" r:id="rId18" display="https://www.crazygames.com/game/shellshockersio" xr:uid="{D974E627-1AAF-42B5-876A-FF9DF261A6A3}"/>
+    <hyperlink ref="C82" r:id="rId19" display="https://www.crazygames.com/game/krunker-io" xr:uid="{51942A3B-7EFC-4C4B-BEE1-7E3470295EA2}"/>
+    <hyperlink ref="C89" r:id="rId20" display="https://www.crazygames.com/game/deadshot-io" xr:uid="{5A03ABEE-6E3A-4526-9F2B-73F0AB9B18BB}"/>
+    <hyperlink ref="C91" r:id="rId21" display="https://www.crazygames.com/game/1v1-lol" xr:uid="{A0BA408D-D347-4BA0-9B94-3BE0B489F493}"/>
+    <hyperlink ref="C92" r:id="rId22" display="https://www.crazygames.com/game/diepio" xr:uid="{B2261812-D809-44FA-A72F-AF1D15359AD4}"/>
+    <hyperlink ref="C84" r:id="rId23" display="https://www.crazygames.com/game/buildroyale-io" xr:uid="{ED0498AB-688F-4EE5-BA70-A6D70EBE3684}"/>
+    <hyperlink ref="C85" r:id="rId24" display="https://www.crazygames.com/game/flyordieio" xr:uid="{382FB2BD-8DEF-405F-BE05-B619F1BB4D1D}"/>
+    <hyperlink ref="C86" r:id="rId25" display="https://www.crazygames.com/game/ducklings" xr:uid="{2424889D-FC6A-4203-AE6A-0D896370241B}"/>
+    <hyperlink ref="C87" r:id="rId26" display="https://www.crazygames.com/game/smash-karts" xr:uid="{CB73B8E1-AECC-4B35-A1AA-5FF59EAF37B2}"/>
+    <hyperlink ref="C88" r:id="rId27" display="https://www.crazygames.com/game/bloxdhop-io" xr:uid="{9BC3A4E9-E8DE-402B-9705-3C34244CCBCD}"/>
+    <hyperlink ref="C90" r:id="rId28" display="https://www.crazygames.com/game/skribblio" xr:uid="{1D9AC806-94C6-44C6-A62E-358D25E6CF23}"/>
+    <hyperlink ref="C83" r:id="rId29" display="https://www.crazygames.com/game/taming-io" xr:uid="{6BAB78B7-B303-4AF1-8CDA-B9A0E30451E2}"/>
     <hyperlink ref="C99" r:id="rId30" display="https://glz.co.il/%D7%92%D7%9C%D7%92%D7%9C%D7%A6" xr:uid="{40BCB9F1-104D-4608-9E1B-A5D35E88203D}"/>
     <hyperlink ref="C96" r:id="rId31" display="https://eco99fm.maariv.co.il/" xr:uid="{F01479AE-4303-4755-92BF-559F63DDDF44}"/>
     <hyperlink ref="C98" r:id="rId32" display="https://103fm.maariv.co.il/" xr:uid="{968AD454-E9F1-4CFE-ACD2-A8E373DED7F6}"/>
@@ -11818,275 +11828,277 @@
     <hyperlink ref="C28" r:id="rId37" xr:uid="{A909ADB7-CEAD-42D0-A603-27F0770BE8C3}"/>
     <hyperlink ref="C27" r:id="rId38" xr:uid="{F78CBC05-5B14-4AA7-B598-DD10E598E62C}"/>
     <hyperlink ref="C26" r:id="rId39" xr:uid="{64BB6B90-35D6-4257-B2DA-47F4C4A3F1A6}"/>
-    <hyperlink ref="C43" r:id="rId40" display="https://us.napster.com" xr:uid="{8D4CC52A-5608-4E3B-91EB-0108BFDB50DA}"/>
-    <hyperlink ref="C51" r:id="rId41" display="https://www.qobuz.com" xr:uid="{CF85F663-80AF-4379-A9D4-E9C587191167}"/>
-    <hyperlink ref="C52" r:id="rId42" display="https://www.idagio.com" xr:uid="{2D48925F-EE1F-4C7D-919B-E473FEC0D720}"/>
-    <hyperlink ref="C63" r:id="rId43" display="https://calmradio.com" xr:uid="{BC594D33-E72A-4BA5-B0B0-E3E7A0CCFD31}"/>
-    <hyperlink ref="C3" r:id="rId44" xr:uid="{62E92066-B899-4BDD-A157-2DB8A685F38B}"/>
-    <hyperlink ref="C4" r:id="rId45" xr:uid="{9F187665-2BE3-46D0-8088-1DBE88E348FE}"/>
-    <hyperlink ref="C5" r:id="rId46" xr:uid="{0A8CD6A4-7D97-4D66-963D-3857FD753A98}"/>
-    <hyperlink ref="C7" r:id="rId47" xr:uid="{D8AC6938-A3EC-41A3-9AFC-A466A245EE24}"/>
-    <hyperlink ref="C94" r:id="rId48" xr:uid="{3FB49C2A-22EE-4315-851C-A8E34FB1ADDF}"/>
-    <hyperlink ref="C8" r:id="rId49" xr:uid="{7C313490-E377-4F1D-B99E-AA798B85C141}"/>
-    <hyperlink ref="C9" r:id="rId50" xr:uid="{9E11F97E-8B26-4B84-9C59-D6EB4A8BA6F1}"/>
-    <hyperlink ref="C10" r:id="rId51" xr:uid="{A6CB0EE3-6E7F-46CC-990E-81E0A57EAD7E}"/>
-    <hyperlink ref="C11" r:id="rId52" xr:uid="{E22B5B9A-82EF-452C-A12C-26305A8DAE27}"/>
-    <hyperlink ref="C13" r:id="rId53" xr:uid="{9F489BDA-D607-4FC7-BAAB-CE91B94A9370}"/>
-    <hyperlink ref="C14" r:id="rId54" xr:uid="{E9344DF6-02F0-48DE-9E6E-7CFE4387A86D}"/>
-    <hyperlink ref="C15" r:id="rId55" xr:uid="{163BDA7C-455A-46BB-9E80-451A9ABF6142}"/>
-    <hyperlink ref="C16" r:id="rId56" xr:uid="{938B0C65-683C-49A0-96EE-CFCBF1C5AB63}"/>
-    <hyperlink ref="C17" r:id="rId57" xr:uid="{E9906A4C-9676-4089-9967-4BB2EFA6646E}"/>
-    <hyperlink ref="C101" r:id="rId58" display="https://courses.campus.gov.il/courses/course-v1:DigitalIsrael+GOV_Oryanut_ExcelBasic101_HE+2022-1/courseware/f6f119b5a0a24fc0a6a4075958245ef7/1fe7c51e6d834517b1ad5003ba140a6d/1?activate_block_id=block-v1%3ADigitalIsrael%2BGOV_Oryanut_ExcelBasic101_HE%2B2022-1%2Btype%40html%2Bblock%40f10d379c29db4e47ae0c6e7e1822c423" xr:uid="{67BF6C12-BC9D-48AC-932D-20E36A5CD01E}"/>
-    <hyperlink ref="C18" r:id="rId59" xr:uid="{463D806D-B86B-4180-9E7F-9EB2BED7841E}"/>
-    <hyperlink ref="C23" r:id="rId60" xr:uid="{4EF2B920-D471-4707-9713-2E599EA07F52}"/>
-    <hyperlink ref="C19" r:id="rId61" xr:uid="{10FC5AF9-9BE7-47D2-887E-5D58C6E8FABC}"/>
-    <hyperlink ref="C20" r:id="rId62" xr:uid="{666E62C8-E82E-4690-B68A-1240E03D1520}"/>
-    <hyperlink ref="C24" r:id="rId63" xr:uid="{4F86FA57-8CF3-4A8A-A74C-2E6BC150EEE4}"/>
-    <hyperlink ref="C30" r:id="rId64" xr:uid="{0A85D764-066B-406E-A867-B93CA0B65FC9}"/>
-    <hyperlink ref="C12" r:id="rId65" location="autoplay" xr:uid="{875E97CE-0FD0-41CD-B187-4B8E7F934150}"/>
+    <hyperlink ref="C50" r:id="rId40" display="https://www.qobuz.com" xr:uid="{CF85F663-80AF-4379-A9D4-E9C587191167}"/>
+    <hyperlink ref="C51" r:id="rId41" display="https://www.idagio.com" xr:uid="{2D48925F-EE1F-4C7D-919B-E473FEC0D720}"/>
+    <hyperlink ref="C62" r:id="rId42" display="https://calmradio.com" xr:uid="{BC594D33-E72A-4BA5-B0B0-E3E7A0CCFD31}"/>
+    <hyperlink ref="C3" r:id="rId43" xr:uid="{62E92066-B899-4BDD-A157-2DB8A685F38B}"/>
+    <hyperlink ref="C4" r:id="rId44" xr:uid="{9F187665-2BE3-46D0-8088-1DBE88E348FE}"/>
+    <hyperlink ref="C5" r:id="rId45" xr:uid="{0A8CD6A4-7D97-4D66-963D-3857FD753A98}"/>
+    <hyperlink ref="C7" r:id="rId46" xr:uid="{D8AC6938-A3EC-41A3-9AFC-A466A245EE24}"/>
+    <hyperlink ref="C94" r:id="rId47" xr:uid="{3FB49C2A-22EE-4315-851C-A8E34FB1ADDF}"/>
+    <hyperlink ref="C9" r:id="rId48" xr:uid="{9E11F97E-8B26-4B84-9C59-D6EB4A8BA6F1}"/>
+    <hyperlink ref="C10" r:id="rId49" xr:uid="{A6CB0EE3-6E7F-46CC-990E-81E0A57EAD7E}"/>
+    <hyperlink ref="C11" r:id="rId50" xr:uid="{E22B5B9A-82EF-452C-A12C-26305A8DAE27}"/>
+    <hyperlink ref="C13" r:id="rId51" xr:uid="{9F489BDA-D607-4FC7-BAAB-CE91B94A9370}"/>
+    <hyperlink ref="C14" r:id="rId52" xr:uid="{E9344DF6-02F0-48DE-9E6E-7CFE4387A86D}"/>
+    <hyperlink ref="C15" r:id="rId53" xr:uid="{163BDA7C-455A-46BB-9E80-451A9ABF6142}"/>
+    <hyperlink ref="C16" r:id="rId54" xr:uid="{938B0C65-683C-49A0-96EE-CFCBF1C5AB63}"/>
+    <hyperlink ref="C17" r:id="rId55" xr:uid="{E9906A4C-9676-4089-9967-4BB2EFA6646E}"/>
+    <hyperlink ref="C101" r:id="rId56" display="https://courses.campus.gov.il/courses/course-v1:DigitalIsrael+GOV_Oryanut_ExcelBasic101_HE+2022-1/courseware/f6f119b5a0a24fc0a6a4075958245ef7/1fe7c51e6d834517b1ad5003ba140a6d/1?activate_block_id=block-v1%3ADigitalIsrael%2BGOV_Oryanut_ExcelBasic101_HE%2B2022-1%2Btype%40html%2Bblock%40f10d379c29db4e47ae0c6e7e1822c423" xr:uid="{67BF6C12-BC9D-48AC-932D-20E36A5CD01E}"/>
+    <hyperlink ref="C18" r:id="rId57" xr:uid="{463D806D-B86B-4180-9E7F-9EB2BED7841E}"/>
+    <hyperlink ref="C23" r:id="rId58" xr:uid="{4EF2B920-D471-4707-9713-2E599EA07F52}"/>
+    <hyperlink ref="C19" r:id="rId59" xr:uid="{10FC5AF9-9BE7-47D2-887E-5D58C6E8FABC}"/>
+    <hyperlink ref="C20" r:id="rId60" xr:uid="{666E62C8-E82E-4690-B68A-1240E03D1520}"/>
+    <hyperlink ref="C24" r:id="rId61" xr:uid="{4F86FA57-8CF3-4A8A-A74C-2E6BC150EEE4}"/>
+    <hyperlink ref="C30" r:id="rId62" xr:uid="{0A85D764-066B-406E-A867-B93CA0B65FC9}"/>
+    <hyperlink ref="C12" r:id="rId63" location="autoplay" xr:uid="{875E97CE-0FD0-41CD-B187-4B8E7F934150}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId66"/>
+  <pageSetup orientation="portrait" r:id="rId64"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FC6163-F89F-44E5-90BE-4CFB44CF1FB4}">
-  <dimension ref="A1:C118"/>
+  <dimension ref="A1:C119"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C1" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>1506</v>
+      </c>
       <c r="C2" s="10" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
-        <v>1289</v>
-      </c>
       <c r="C3" s="10" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" s="10" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" s="10" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" s="10" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="10" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" s="10" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" s="10" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" s="10" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" s="10" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" s="10" t="s">
-        <v>951</v>
+        <v>962</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" s="10" t="s">
-        <v>962</v>
+        <v>953</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" s="10" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" s="10" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="10" t="s">
-        <v>955</v>
+        <v>963</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="10" t="s">
-        <v>963</v>
+        <v>956</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="10" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="10" t="s">
-        <v>957</v>
+      <c r="C20" s="2" t="s">
+        <v>923</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="2" t="s">
-        <v>923</v>
+      <c r="C21" s="10" t="s">
+        <v>958</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="10" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="10" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" s="10" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="10" t="s">
-        <v>961</v>
+      <c r="C25" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>935</v>
+        <v>915</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>918</v>
+        <v>929</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>929</v>
+        <v>882</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>882</v>
+        <v>887</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>887</v>
+        <v>893</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>893</v>
+        <v>904</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>904</v>
+        <v>908</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>913</v>
+        <v>878</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>879</v>
+        <v>865</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>868</v>
+      <c r="C42" s="16" t="s">
+        <v>970</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C43" s="16" t="s">
-        <v>970</v>
+      <c r="C43" s="10" t="s">
+        <v>939</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" s="10" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.25">
@@ -12094,7 +12106,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="9" t="s">
         <v>699</v>
       </c>
@@ -12459,9 +12471,14 @@
         <v>952</v>
       </c>
     </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>875</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{63F314B8-DBD1-404D-ADDB-F1388B3579E5}"/>
+    <hyperlink ref="C44" r:id="rId1" xr:uid="{63F314B8-DBD1-404D-ADDB-F1388B3579E5}"/>
     <hyperlink ref="C108" r:id="rId2" xr:uid="{C28D3562-05A2-4373-A0F6-04979F955C69}"/>
     <hyperlink ref="C109" r:id="rId3" xr:uid="{74BDD072-1C24-4024-A8A3-52C22DC4F4AE}"/>
     <hyperlink ref="C110" r:id="rId4" xr:uid="{574FC8C6-AE4C-4915-B344-24B73E82B9F9}"/>
@@ -12532,7 +12549,7 @@
     <hyperlink ref="C95" r:id="rId69" xr:uid="{455178C1-F175-4580-B052-8E6DE4D7ECAD}"/>
     <hyperlink ref="C96" r:id="rId70" xr:uid="{E287708F-2FC6-4C0F-B23B-FC0F1609F7A0}"/>
     <hyperlink ref="C97" r:id="rId71" xr:uid="{A8465678-1427-486F-BEAC-27B7BF15EF20}"/>
-    <hyperlink ref="C21" r:id="rId72" xr:uid="{6A0FBB2A-F01F-4F12-A2A2-84B3093329DD}"/>
+    <hyperlink ref="C20" r:id="rId72" xr:uid="{6A0FBB2A-F01F-4F12-A2A2-84B3093329DD}"/>
     <hyperlink ref="C117" r:id="rId73" xr:uid="{BA1FD2BE-D270-4B76-9A7B-B63DEDA3EB5B}"/>
     <hyperlink ref="C116" r:id="rId74" xr:uid="{29507CAC-4255-40A4-A2F4-82B3EB3ADCC6}"/>
   </hyperlinks>
@@ -12553,13 +12570,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C1" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -13079,13 +13096,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C1" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -13619,13 +13636,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C1" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -14454,13 +14471,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C1" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
audio 59 sites check
</commit_message>
<xml_diff>
--- a/Crawler/App_direct_links.xlsx
+++ b/Crawler/App_direct_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Desktop\Final_Project\Crawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F600DFE1-A802-4B72-A327-2524C20DEBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD23023A-4746-4594-91E3-0B0BDBB9889C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="975" windowWidth="12810" windowHeight="12000" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FINAL" sheetId="16" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2051" uniqueCount="1546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="1585">
   <si>
     <t>Khan Academy</t>
   </si>
@@ -4661,9 +4661,6 @@
     <t>play</t>
   </si>
   <si>
-    <t>sp_choice_type_11,button_play</t>
-  </si>
-  <si>
     <t>shadowRoot</t>
   </si>
   <si>
@@ -4683,13 +4680,133 @@
   </si>
   <si>
     <t>play-pause</t>
+  </si>
+  <si>
+    <t>vjs-play-control</t>
+  </si>
+  <si>
+    <t>shoutcast779playbutton</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/show/6TMepIcA0MjQm96IFzvK08</t>
+  </si>
+  <si>
+    <t>e-9960-button-icon-only--small</t>
+  </si>
+  <si>
+    <t>episode-play-button</t>
+  </si>
+  <si>
+    <t>sp_choice_type_11,PlayButton_buttonWrapper___CMG4</t>
+  </si>
+  <si>
+    <t>https://www.kan.org.il/content/kan/podcasts/p-8127/922873/</t>
+  </si>
+  <si>
+    <t>audio-player-play-btn</t>
+  </si>
+  <si>
+    <t>https://1045fm.maariv.co.il/programs/media.aspx?ZrqvnVq=IMKHLE&amp;c41t4nzVQ=EFGM</t>
+  </si>
+  <si>
+    <t>mouthjs-playbutton</t>
+  </si>
+  <si>
+    <t>https://1075.fm/popup-player/?curtrack=552</t>
+  </si>
+  <si>
+    <t>radio-play-btn</t>
+  </si>
+  <si>
+    <t>radio-play-pause</t>
+  </si>
+  <si>
+    <t>qw-playerbutton</t>
+  </si>
+  <si>
+    <t>menu-item-406</t>
+  </si>
+  <si>
+    <t>https://www.emess.co.il/audio/program/525</t>
+  </si>
+  <si>
+    <t>icon-play</t>
+  </si>
+  <si>
+    <t>https://radio.streamgates.net/stream/101fm</t>
+  </si>
+  <si>
+    <t>http://live1.co.il/jrs101fm/</t>
+  </si>
+  <si>
+    <t>play-button-container</t>
+  </si>
+  <si>
+    <t>https://gly.co.il/item?id=39462</t>
+  </si>
+  <si>
+    <t>popup_close,seg_play</t>
+  </si>
+  <si>
+    <t>noSelect</t>
+  </si>
+  <si>
+    <t>iconWrapper</t>
+  </si>
+  <si>
+    <t>https://eco99fm.maariv.co.il/live-radio</t>
+  </si>
+  <si>
+    <t>play-btn</t>
+  </si>
+  <si>
+    <t>https://103fm.maariv.co.il/programs/media.aspx?ZrqvnVq=JMKGDJ&amp;c41t4nzVQ=JKF</t>
+  </si>
+  <si>
+    <t>css-18o0txe</t>
+  </si>
+  <si>
+    <t>https://www.995.co.il/popup-player</t>
+  </si>
+  <si>
+    <t>jp-play</t>
+  </si>
+  <si>
+    <t>https://glz.co.il/%D7%92%D7%9C%D7%A6/%D7%AA%D7%95%D7%9B%D7%A0%D7%99%D7%95%D7%AA/%D7%97%D7%99%D7%99%D7%9D-%D7%A9%D7%9C-%D7%90%D7%97%D7%A8%D7%99%D7%9D</t>
+  </si>
+  <si>
+    <t>btn_234613</t>
+  </si>
+  <si>
+    <t>https://www.100fm.co.il/program/%d7%a4%d7%a8%d7%99%d7%a9%d7%94-%d7%91%d7%a7%d7%9c%d7%99%d7%a7/</t>
+  </si>
+  <si>
+    <t>https://www.1036kh.com/podcast/episode/2f091908</t>
+  </si>
+  <si>
+    <t>s__3b64FT</t>
+  </si>
+  <si>
+    <t>mejs__overlay-button</t>
+  </si>
+  <si>
+    <t>https://www.bbc.co.uk/sounds/play/live/bbc_radio_one</t>
+  </si>
+  <si>
+    <t>p_audioui_playpause</t>
+  </si>
+  <si>
+    <t>onetrust-accept-btn-handler,pn-modal__button,audio-module-listen</t>
+  </si>
+  <si>
+    <t>https://www.npr.org/2025/06/18/1254350237/the-npr-politics-podcast-iran-israel-trump-maga</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4753,6 +4870,13 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF211A1D"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -4805,7 +4929,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -4853,6 +4977,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11718,10 +11844,10 @@
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
@@ -11975,10 +12101,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FC6163-F89F-44E5-90BE-4CFB44CF1FB4}">
-  <dimension ref="A1:C118"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11990,7 +12116,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="B1" t="s">
         <v>1289</v>
@@ -12003,7 +12129,7 @@
       <c r="B2" s="20" t="s">
         <v>1502</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>940</v>
       </c>
     </row>
@@ -12011,7 +12137,7 @@
       <c r="B3" s="18" t="s">
         <v>1504</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>941</v>
       </c>
     </row>
@@ -12019,7 +12145,7 @@
       <c r="B4" s="18" t="s">
         <v>1505</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>943</v>
       </c>
     </row>
@@ -12027,7 +12153,7 @@
       <c r="B5" t="s">
         <v>1506</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>944</v>
       </c>
     </row>
@@ -12038,7 +12164,7 @@
       <c r="B6" s="18" t="s">
         <v>1507</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>945</v>
       </c>
     </row>
@@ -12046,7 +12172,7 @@
       <c r="B7" t="s">
         <v>1508</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>946</v>
       </c>
     </row>
@@ -12054,7 +12180,7 @@
       <c r="B8" s="18" t="s">
         <v>1509</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>947</v>
       </c>
     </row>
@@ -12062,7 +12188,7 @@
       <c r="B9" s="18" t="s">
         <v>1510</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>948</v>
       </c>
     </row>
@@ -12070,7 +12196,7 @@
       <c r="B10" s="18" t="s">
         <v>1511</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>949</v>
       </c>
     </row>
@@ -12078,7 +12204,7 @@
       <c r="B11" s="18" t="s">
         <v>1512</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>950</v>
       </c>
     </row>
@@ -12086,7 +12212,7 @@
       <c r="B12" s="18" t="s">
         <v>1513</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>951</v>
       </c>
     </row>
@@ -12094,7 +12220,7 @@
       <c r="B13" s="18" t="s">
         <v>1514</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>953</v>
       </c>
     </row>
@@ -12102,7 +12228,7 @@
       <c r="B14" t="s">
         <v>1515</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>954</v>
       </c>
     </row>
@@ -12110,7 +12236,7 @@
       <c r="B15" s="18" t="s">
         <v>1516</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>955</v>
       </c>
     </row>
@@ -12118,7 +12244,7 @@
       <c r="B16" s="18" t="s">
         <v>1517</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>963</v>
       </c>
     </row>
@@ -12126,7 +12252,7 @@
       <c r="B17" s="18" t="s">
         <v>1518</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>956</v>
       </c>
     </row>
@@ -12134,7 +12260,7 @@
       <c r="B18" t="s">
         <v>1519</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>957</v>
       </c>
     </row>
@@ -12142,7 +12268,7 @@
       <c r="B19" s="18" t="s">
         <v>1523</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="9" t="s">
         <v>923</v>
       </c>
     </row>
@@ -12150,7 +12276,7 @@
       <c r="B20" s="18" t="s">
         <v>1524</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>958</v>
       </c>
     </row>
@@ -12158,7 +12284,7 @@
       <c r="B21" s="18" t="s">
         <v>1525</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>959</v>
       </c>
     </row>
@@ -12166,7 +12292,7 @@
       <c r="B22" s="18" t="s">
         <v>1526</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>960</v>
       </c>
     </row>
@@ -12174,7 +12300,7 @@
       <c r="B23" s="18" t="s">
         <v>1528</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>1527</v>
       </c>
     </row>
@@ -12182,7 +12308,7 @@
       <c r="B24" s="18" t="s">
         <v>1529</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="5" t="s">
         <v>931</v>
       </c>
     </row>
@@ -12190,7 +12316,7 @@
       <c r="B25" s="18" t="s">
         <v>1530</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="5" t="s">
         <v>933</v>
       </c>
     </row>
@@ -12198,12 +12324,12 @@
       <c r="B26" s="18" t="s">
         <v>1531</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="5" t="s">
         <v>915</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+      <c r="C27" s="5" t="s">
         <v>918</v>
       </c>
     </row>
@@ -12211,7 +12337,7 @@
       <c r="B28" s="18" t="s">
         <v>1532</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="5" t="s">
         <v>929</v>
       </c>
     </row>
@@ -12222,7 +12348,7 @@
       <c r="B29" s="18" t="s">
         <v>1533</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="5" t="s">
         <v>882</v>
       </c>
     </row>
@@ -12230,7 +12356,7 @@
       <c r="B30" s="18" t="s">
         <v>1536</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="5" t="s">
         <v>887</v>
       </c>
     </row>
@@ -12238,542 +12364,421 @@
       <c r="B31" s="18" t="s">
         <v>1537</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="5" t="s">
         <v>893</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="18" t="s">
-        <v>1538</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1541</v>
+        <v>1550</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>1540</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>1524</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="5" t="s">
         <v>908</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
-        <v>1544</v>
-      </c>
-      <c r="C34" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
+        <v>1544</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="18" t="s">
         <v>1545</v>
       </c>
-      <c r="C35" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>878</v>
+      <c r="C36" s="5" t="s">
+        <v>865</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>879</v>
+      <c r="B37" s="18" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>970</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>865</v>
+      <c r="B38" s="18" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>1547</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>868</v>
+      <c r="B39" s="18" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>972</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C40" s="15" t="s">
-        <v>970</v>
+      <c r="B40" s="18" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C41" s="10" t="s">
-        <v>939</v>
+      <c r="B41" s="18" t="s">
+        <v>1554</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>1553</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C42" s="10" t="s">
+      <c r="B42" s="25" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="18" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="18" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="18" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="18" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="18" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="18"/>
+      <c r="C48" s="9" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="18" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="18" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="18" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="18" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="18" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="18" t="s">
+        <v>1572</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="18" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="18" t="s">
+        <v>1576</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="18" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="18" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="18" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="18" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="18" t="s">
+        <v>1583</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="10" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="10" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="10" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="10" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="10" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="10" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="10" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="10" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="10" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="10" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="10" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="12" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="12" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="12" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="12" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="12" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="12" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="12" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="12" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="12" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="12" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="13" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="23" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="10" t="s">
         <v>938</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C43" s="15" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="9" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C45" s="9" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C46" s="9" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C47" s="9" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C48" s="9" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" s="9" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" s="9" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51" s="9" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C52" s="9" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53" s="9" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" s="9" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C55" s="9" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C56" s="9" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C57" s="9" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C58" s="9" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C59" s="9" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C60" s="9" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C61" s="9" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C62" s="9" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C63" s="9" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C64" s="9" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65" s="9" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C66" s="9" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C67" s="9" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C68" s="9" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C69" s="9" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C70" s="9" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C71" s="9" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C72" s="9" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C73" s="9" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C74" s="9" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C75" s="9" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C76" s="9" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C77" s="9" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C78" s="9" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C79" s="9" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C80" s="9" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81" s="9" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C82" s="9" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C83" s="9" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C84" s="9" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C85" s="9" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C86" s="9" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C87" s="9" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C88" s="9" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C89" s="9" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C90" s="9" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C91" s="9" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C92" s="9" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C93" s="9" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C94" s="9" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C95" s="9" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C96" s="9" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C97" s="9" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C98" s="9" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C99" s="9" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C100" s="9" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C101" s="9" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C102" s="9" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C103" s="9" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C104" s="9" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C105" s="9" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C106" s="12" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C107" s="12" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C108" s="12" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C109" s="12" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C110" s="12" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C111" s="12" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C112" s="12" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C113" s="12" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C114" s="12" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C115" s="12" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C116" s="13" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C117" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C118" s="23" t="s">
-        <v>888</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C42" r:id="rId1" xr:uid="{63F314B8-DBD1-404D-ADDB-F1388B3579E5}"/>
-    <hyperlink ref="C106" r:id="rId2" xr:uid="{C28D3562-05A2-4373-A0F6-04979F955C69}"/>
-    <hyperlink ref="C107" r:id="rId3" xr:uid="{74BDD072-1C24-4024-A8A3-52C22DC4F4AE}"/>
-    <hyperlink ref="C108" r:id="rId4" xr:uid="{574FC8C6-AE4C-4915-B344-24B73E82B9F9}"/>
-    <hyperlink ref="C109" r:id="rId5" xr:uid="{61044818-0939-4A90-8599-B2A568594274}"/>
-    <hyperlink ref="C110" r:id="rId6" xr:uid="{C75D6396-175B-4AB6-9D50-BEEF6413E95D}"/>
-    <hyperlink ref="C111" r:id="rId7" xr:uid="{32731225-C97F-44A3-81C0-6BB3D5561589}"/>
-    <hyperlink ref="C113" r:id="rId8" xr:uid="{9A4C38CF-C385-46C4-AF5E-4BD5C83ADECD}"/>
-    <hyperlink ref="C112" r:id="rId9" xr:uid="{317D8014-D715-4187-93BD-408899CC13ED}"/>
-    <hyperlink ref="C44" r:id="rId10" xr:uid="{CACF3F4B-FD60-4F5D-80DE-4F989827283B}"/>
-    <hyperlink ref="C45" r:id="rId11" xr:uid="{B621D8DE-A767-4BBD-BE22-640A75CA5D91}"/>
-    <hyperlink ref="C46" r:id="rId12" xr:uid="{E343DF28-D7C6-487D-8890-421CD37C42EB}"/>
-    <hyperlink ref="C47" r:id="rId13" xr:uid="{393CD1D9-6D85-43AC-847D-1BF2CF74E366}"/>
-    <hyperlink ref="C48" r:id="rId14" xr:uid="{E118AE26-9368-4DE4-9299-26E63628339C}"/>
-    <hyperlink ref="C49" r:id="rId15" xr:uid="{D0393A7E-EC42-4E0E-A98F-C8F2B2386DB9}"/>
-    <hyperlink ref="C50" r:id="rId16" xr:uid="{45CA9E57-58A2-4669-B92E-D18354127A7A}"/>
-    <hyperlink ref="C51" r:id="rId17" xr:uid="{D8BD5A9B-DC4B-4A04-ACC9-F2A1BEA9D332}"/>
-    <hyperlink ref="C52" r:id="rId18" xr:uid="{04F0B8E6-39DE-4116-A66A-09152BBF7CA1}"/>
-    <hyperlink ref="C53" r:id="rId19" xr:uid="{0042D724-A44C-49DB-8C11-798623C9F02E}"/>
-    <hyperlink ref="C54" r:id="rId20" xr:uid="{82C2869E-FB63-4D88-8258-85F9BF076209}"/>
-    <hyperlink ref="C55" r:id="rId21" xr:uid="{1102FEC3-A4A2-4B0F-ADE4-3D751ECF38FC}"/>
-    <hyperlink ref="C56" r:id="rId22" xr:uid="{C21D3D86-1F2D-4E8D-A7CB-5189D8F456B6}"/>
-    <hyperlink ref="C57" r:id="rId23" xr:uid="{CFCDD53B-868B-4558-87DA-9621CCBB313F}"/>
-    <hyperlink ref="C58" r:id="rId24" xr:uid="{7F7B17FD-BE50-4A04-835D-927E484FB8E1}"/>
-    <hyperlink ref="C59" r:id="rId25" xr:uid="{6C5A4EE0-E514-4B33-BA2B-26BB5453FE55}"/>
-    <hyperlink ref="C60" r:id="rId26" xr:uid="{9F0AA92C-C581-4FB2-88BD-43045313725E}"/>
-    <hyperlink ref="C61" r:id="rId27" xr:uid="{40C9C721-A72B-4760-ACE3-E8AD6E343AF9}"/>
-    <hyperlink ref="C62" r:id="rId28" xr:uid="{6ED252E3-1A5A-463F-B8CA-EE5F62CFF274}"/>
-    <hyperlink ref="C63" r:id="rId29" xr:uid="{CE17CEF1-9490-446E-A22A-B4C8A5DB656A}"/>
-    <hyperlink ref="C64" r:id="rId30" xr:uid="{E1A24C18-823A-4306-8077-9A5DC1EA092E}"/>
-    <hyperlink ref="C65" r:id="rId31" xr:uid="{2F0B5BB0-87DC-43D1-BACB-384A98AFF5C1}"/>
-    <hyperlink ref="C66" r:id="rId32" xr:uid="{89FB00D7-0299-4541-AD03-9354C18AE10A}"/>
-    <hyperlink ref="C67" r:id="rId33" xr:uid="{D101A818-34FE-4E2E-B70F-64BB3B0AA327}"/>
-    <hyperlink ref="C68" r:id="rId34" xr:uid="{768B14C4-770A-4C55-8FA2-AC356966313C}"/>
-    <hyperlink ref="C69" r:id="rId35" xr:uid="{DA258324-2BCB-404B-8CAD-1C4F7D9C69F0}"/>
-    <hyperlink ref="C70" r:id="rId36" xr:uid="{4E66D9A3-1977-49B0-8CE0-D772D9935E89}"/>
-    <hyperlink ref="C71" r:id="rId37" xr:uid="{37AC3147-1434-402A-AE31-2D0AE7521865}"/>
-    <hyperlink ref="C105" r:id="rId38" xr:uid="{CCD0B607-4738-4A9C-BEF5-9EC39695453C}"/>
-    <hyperlink ref="C104" r:id="rId39" xr:uid="{698B805A-481F-4BFE-B2E0-9B35F29E394B}"/>
-    <hyperlink ref="C103" r:id="rId40" xr:uid="{603DC9C9-06BB-4EDB-AFCD-C9AFC97A49FB}"/>
-    <hyperlink ref="C102" r:id="rId41" xr:uid="{8A64217F-DDBB-43C6-A6CB-41860C8EC627}"/>
-    <hyperlink ref="C101" r:id="rId42" xr:uid="{54E96382-8196-4BE4-B827-1C21138A8EBB}"/>
-    <hyperlink ref="C100" r:id="rId43" xr:uid="{19C0620A-A37A-4414-BEBA-FA224D4D1248}"/>
-    <hyperlink ref="C99" r:id="rId44" xr:uid="{DD7D960F-E485-4EB0-8C3C-658FF1E7C791}"/>
-    <hyperlink ref="C98" r:id="rId45" xr:uid="{DAEC30C9-1203-405A-92E7-934BB88B171E}"/>
-    <hyperlink ref="C97" r:id="rId46" xr:uid="{954D9F3A-F840-4C59-AFA6-A6722F3F256D}"/>
-    <hyperlink ref="C96" r:id="rId47" xr:uid="{DC52B000-1FC8-4907-909D-B434FC0591BC}"/>
-    <hyperlink ref="C72" r:id="rId48" xr:uid="{EC7E067B-B344-4215-B67F-066FFF3BB015}"/>
-    <hyperlink ref="C73" r:id="rId49" xr:uid="{3064A639-44E8-462A-B8B8-199B2145DA6A}"/>
-    <hyperlink ref="C74" r:id="rId50" xr:uid="{5F90A03D-704E-4363-B6C5-77E374A4C34C}"/>
-    <hyperlink ref="C75" r:id="rId51" xr:uid="{B2669C5D-06DE-4B76-9ED8-B7AD33812FAB}"/>
-    <hyperlink ref="C76" r:id="rId52" xr:uid="{EB935972-5A53-4EFE-B2ED-28DB075FF785}"/>
-    <hyperlink ref="C77" r:id="rId53" xr:uid="{82F21A45-69D3-4AFD-BAB6-F70E65634772}"/>
-    <hyperlink ref="C78" r:id="rId54" xr:uid="{3FE44C2B-044D-487D-99C7-CC11FD84EC70}"/>
-    <hyperlink ref="C79" r:id="rId55" xr:uid="{91662DE5-36FC-426A-BE97-2CF289DAA7E8}"/>
-    <hyperlink ref="C80" r:id="rId56" xr:uid="{F80B58BD-AE57-4872-8B78-9642CC138842}"/>
-    <hyperlink ref="C81" r:id="rId57" xr:uid="{EB15B0CA-38C8-4F63-AB4B-E2DCF42B030F}"/>
-    <hyperlink ref="C82" r:id="rId58" xr:uid="{209C6D8B-8EEF-4D33-A631-7B5200F2A7BC}"/>
-    <hyperlink ref="C83" r:id="rId59" xr:uid="{40C460FF-5039-45A0-9990-F58B898CC5D2}"/>
-    <hyperlink ref="C84" r:id="rId60" xr:uid="{D5C94AA2-457D-4EB3-9757-17E119BED846}"/>
-    <hyperlink ref="C85" r:id="rId61" xr:uid="{9A475341-5F99-4792-9D5B-EDE04D483C0F}"/>
-    <hyperlink ref="C86" r:id="rId62" xr:uid="{8E7485E5-7083-4D39-B2B8-82FB0DEFD5D3}"/>
-    <hyperlink ref="C87" r:id="rId63" xr:uid="{AF5B7AEA-2C18-4DCB-8319-296AF51ABD74}"/>
-    <hyperlink ref="C88" r:id="rId64" xr:uid="{F4F44B7B-7022-4C8C-A971-B9C7F106916A}"/>
-    <hyperlink ref="C89" r:id="rId65" xr:uid="{A4D574C0-F69B-47B4-B6BE-24BD59B1F37E}"/>
-    <hyperlink ref="C90" r:id="rId66" xr:uid="{725F13E7-12CF-42E8-B98B-9EA63EB5FE2D}"/>
-    <hyperlink ref="C91" r:id="rId67" xr:uid="{98547F72-A493-4133-8857-2EC85CD29A2D}"/>
-    <hyperlink ref="C92" r:id="rId68" xr:uid="{1AD42A18-5C6A-469C-984A-68CA68C03474}"/>
-    <hyperlink ref="C93" r:id="rId69" xr:uid="{455178C1-F175-4580-B052-8E6DE4D7ECAD}"/>
-    <hyperlink ref="C94" r:id="rId70" xr:uid="{E287708F-2FC6-4C0F-B23B-FC0F1609F7A0}"/>
-    <hyperlink ref="C95" r:id="rId71" xr:uid="{A8465678-1427-486F-BEAC-27B7BF15EF20}"/>
-    <hyperlink ref="C19" r:id="rId72" xr:uid="{6A0FBB2A-F01F-4F12-A2A2-84B3093329DD}"/>
-    <hyperlink ref="C115" r:id="rId73" xr:uid="{BA1FD2BE-D270-4B76-9A7B-B63DEDA3EB5B}"/>
-    <hyperlink ref="C114" r:id="rId74" xr:uid="{29507CAC-4255-40A4-A2F4-82B3EB3ADCC6}"/>
-    <hyperlink ref="C6" r:id="rId75" xr:uid="{749FF0BD-4C6F-42EA-AB65-D92A352CDA58}"/>
-    <hyperlink ref="C7" r:id="rId76" xr:uid="{5646E514-FD80-400A-861F-C88E87997722}"/>
-    <hyperlink ref="C118" r:id="rId77" xr:uid="{7F58F8A6-F514-49E8-9F1F-7AD7BCF776D7}"/>
+    <hyperlink ref="C86" r:id="rId1" xr:uid="{63F314B8-DBD1-404D-ADDB-F1388B3579E5}"/>
+    <hyperlink ref="C73" r:id="rId2" xr:uid="{C28D3562-05A2-4373-A0F6-04979F955C69}"/>
+    <hyperlink ref="C74" r:id="rId3" xr:uid="{74BDD072-1C24-4024-A8A3-52C22DC4F4AE}"/>
+    <hyperlink ref="C75" r:id="rId4" xr:uid="{574FC8C6-AE4C-4915-B344-24B73E82B9F9}"/>
+    <hyperlink ref="C76" r:id="rId5" xr:uid="{61044818-0939-4A90-8599-B2A568594274}"/>
+    <hyperlink ref="C77" r:id="rId6" xr:uid="{C75D6396-175B-4AB6-9D50-BEEF6413E95D}"/>
+    <hyperlink ref="C78" r:id="rId7" xr:uid="{32731225-C97F-44A3-81C0-6BB3D5561589}"/>
+    <hyperlink ref="C80" r:id="rId8" xr:uid="{9A4C38CF-C385-46C4-AF5E-4BD5C83ADECD}"/>
+    <hyperlink ref="C79" r:id="rId9" xr:uid="{317D8014-D715-4187-93BD-408899CC13ED}"/>
+    <hyperlink ref="C43" r:id="rId10" xr:uid="{D8BD5A9B-DC4B-4A04-ACC9-F2A1BEA9D332}"/>
+    <hyperlink ref="C44" r:id="rId11" xr:uid="{1102FEC3-A4A2-4B0F-ADE4-3D751ECF38FC}"/>
+    <hyperlink ref="C45" r:id="rId12" xr:uid="{C21D3D86-1F2D-4E8D-A7CB-5189D8F456B6}"/>
+    <hyperlink ref="C51" r:id="rId13" xr:uid="{40C9C721-A72B-4760-ACE3-E8AD6E343AF9}"/>
+    <hyperlink ref="C52" r:id="rId14" xr:uid="{6ED252E3-1A5A-463F-B8CA-EE5F62CFF274}"/>
+    <hyperlink ref="C72" r:id="rId15" xr:uid="{CCD0B607-4738-4A9C-BEF5-9EC39695453C}"/>
+    <hyperlink ref="C71" r:id="rId16" xr:uid="{698B805A-481F-4BFE-B2E0-9B35F29E394B}"/>
+    <hyperlink ref="C70" r:id="rId17" xr:uid="{603DC9C9-06BB-4EDB-AFCD-C9AFC97A49FB}"/>
+    <hyperlink ref="C69" r:id="rId18" xr:uid="{8A64217F-DDBB-43C6-A6CB-41860C8EC627}"/>
+    <hyperlink ref="C68" r:id="rId19" xr:uid="{54E96382-8196-4BE4-B827-1C21138A8EBB}"/>
+    <hyperlink ref="C67" r:id="rId20" xr:uid="{19C0620A-A37A-4414-BEBA-FA224D4D1248}"/>
+    <hyperlink ref="C66" r:id="rId21" xr:uid="{DD7D960F-E485-4EB0-8C3C-658FF1E7C791}"/>
+    <hyperlink ref="C65" r:id="rId22" xr:uid="{DAEC30C9-1203-405A-92E7-934BB88B171E}"/>
+    <hyperlink ref="C64" r:id="rId23" xr:uid="{954D9F3A-F840-4C59-AFA6-A6722F3F256D}"/>
+    <hyperlink ref="C63" r:id="rId24" xr:uid="{DC52B000-1FC8-4907-909D-B434FC0591BC}"/>
+    <hyperlink ref="C59" r:id="rId25" xr:uid="{1AD42A18-5C6A-469C-984A-68CA68C03474}"/>
+    <hyperlink ref="C62" r:id="rId26" xr:uid="{A8465678-1427-486F-BEAC-27B7BF15EF20}"/>
+    <hyperlink ref="C19" r:id="rId27" xr:uid="{6A0FBB2A-F01F-4F12-A2A2-84B3093329DD}"/>
+    <hyperlink ref="C82" r:id="rId28" xr:uid="{BA1FD2BE-D270-4B76-9A7B-B63DEDA3EB5B}"/>
+    <hyperlink ref="C81" r:id="rId29" xr:uid="{29507CAC-4255-40A4-A2F4-82B3EB3ADCC6}"/>
+    <hyperlink ref="C6" r:id="rId30" xr:uid="{749FF0BD-4C6F-42EA-AB65-D92A352CDA58}"/>
+    <hyperlink ref="C7" r:id="rId31" xr:uid="{5646E514-FD80-400A-861F-C88E87997722}"/>
+    <hyperlink ref="C85" r:id="rId32" xr:uid="{7F58F8A6-F514-49E8-9F1F-7AD7BCF776D7}"/>
+    <hyperlink ref="C37" r:id="rId33" xr:uid="{E815B360-D8AF-4CCE-9CED-F2C672B9729D}"/>
+    <hyperlink ref="C41" r:id="rId34" xr:uid="{86C497B9-5A0E-4A31-84E4-36040284A197}"/>
+    <hyperlink ref="C46" r:id="rId35" xr:uid="{CFCDD53B-868B-4558-87DA-9621CCBB313F}"/>
+    <hyperlink ref="C48" r:id="rId36" xr:uid="{364A8617-AF30-4696-8915-C49811E408BC}"/>
+    <hyperlink ref="C50" r:id="rId37" xr:uid="{49F841D7-7E05-4BC4-B96C-B2D651A60799}"/>
+    <hyperlink ref="C55" r:id="rId38" xr:uid="{029DBA7B-42D5-4D7B-ACD0-4722509BC974}"/>
+    <hyperlink ref="C42" r:id="rId39" xr:uid="{D7452DF6-F577-4F68-898F-87018A9F90E3}"/>
+    <hyperlink ref="C60" r:id="rId40" xr:uid="{E57511F6-433E-4C0A-9E55-A6D616B4B542}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId78"/>
+  <pageSetup orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
switching orange links part 1
</commit_message>
<xml_diff>
--- a/Crawler/App_direct_links.xlsx
+++ b/Crawler/App_direct_links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\פרויקט גמר\network_traffic_project\Crawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBEFF26-6050-42E6-B76B-CCE73ADD7DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E08FEF-820D-4F23-9912-991E83B9482E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="1659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="1696">
   <si>
     <t>Khan Academy</t>
   </si>
@@ -4562,9 +4562,6 @@
     <t>https://almalinux.org/get-almalinux/</t>
   </si>
   <si>
-    <t>itemAl_01</t>
-  </si>
-  <si>
     <t>https://www.learningcontainer.com/download/sample-pdf-file-for-testing/</t>
   </si>
   <si>
@@ -4640,9 +4637,6 @@
     <t>w</t>
   </si>
   <si>
-    <t>https://www.fosshub.com/1by1.html</t>
-  </si>
-  <si>
     <t>https://gamejolt.com/app</t>
   </si>
   <si>
@@ -4838,9 +4832,6 @@
     <t>https://commons.wikimedia.org/wiki/Category:3D_city_models#/media/File:2019_City_of_London_3D_model.jpg</t>
   </si>
   <si>
-    <t>https://en.wikisource.org/wiki/A_Pipe_of_Tobacco</t>
-  </si>
-  <si>
     <t>ui.compact.mini.button</t>
   </si>
   <si>
@@ -4853,15 +4844,6 @@
     <t>https://archive.org/details/lmc-8.4-r-8</t>
   </si>
   <si>
-    <t>download-btn</t>
-  </si>
-  <si>
-    <t>https://librivox.org/author/5940?primary_key=5940&amp;search_category=author&amp;search_page=1&amp;search_form=get_results&amp;search_order=alpha</t>
-  </si>
-  <si>
-    <t>https://openlibrary.org/</t>
-  </si>
-  <si>
     <t>https://www.freepik.com/free-photo/young-woman-teacher-wearing-glasses-explaining-lesson-holding-stack-books-looking-confident-standing-school-desk-front-blackboard-classroom_26397314.htm#fromView=keyword&amp;page=1&amp;position=2&amp;uuid=f2d9c8ff-4958-4fdf-a220-d39d4c853740&amp;from_element=categories_trends&amp;query=University+Teacher</t>
   </si>
   <si>
@@ -4880,9 +4862,6 @@
     <t>https://www.jamendo.com/</t>
   </si>
   <si>
-    <t>https://bandcamp.com/</t>
-  </si>
-  <si>
     <t>https://datpiff.com/</t>
   </si>
   <si>
@@ -4961,9 +4940,6 @@
     <t>https://openclipart.org/detail/351987/only-love</t>
   </si>
   <si>
-    <t>http://www.clker.com/</t>
-  </si>
-  <si>
     <t>.btn.btn-green.btn-lg</t>
   </si>
   <si>
@@ -5022,6 +4998,141 @@
   </si>
   <si>
     <t>https://licensing.jamendo.com/en</t>
+  </si>
+  <si>
+    <t>book-download-btn</t>
+  </si>
+  <si>
+    <t>https://librivox.org/transient-by-ward-moore/</t>
+  </si>
+  <si>
+    <t>https://www.fosshub.com/3uTools.html</t>
+  </si>
+  <si>
+    <t>downloadButtonSubtitle</t>
+  </si>
+  <si>
+    <t>https://www.apkmirror.com/apk/google-inc/maps/google-maps-25-26-01-774458481-release/google-maps-25-26-01-774458481-android-apk-download/</t>
+  </si>
+  <si>
+    <t>.nav-link.btn.btn.al-download-button</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>https://www.7-zip.org/</t>
+  </si>
+  <si>
+    <t>https://archlinux.org/download/</t>
+  </si>
+  <si>
+    <t>Download.torrent</t>
+  </si>
+  <si>
+    <t>https://www.win-rar.com/download.html?&amp;L=0</t>
+  </si>
+  <si>
+    <t>dwn-btn</t>
+  </si>
+  <si>
+    <t>https://www.python.org/downloads/</t>
+  </si>
+  <si>
+    <t>download-buttons</t>
+  </si>
+  <si>
+    <t>.btn.btn-primary.btn-sm</t>
+  </si>
+  <si>
+    <t>https://incompetech.com/music/royalty-free/index.html?isrc=USUAN1200067&amp;Search=Search</t>
+  </si>
+  <si>
+    <t>.format-summary.download-pill</t>
+  </si>
+  <si>
+    <t>https://archive.org/details/dn2025-0625_vid</t>
+  </si>
+  <si>
+    <t>https://ocw.mit.edu/courses/res-18-010-a-2020-vision-of-linear-algebra-spring-2020/download/</t>
+  </si>
+  <si>
+    <t>download-course-button.p-2</t>
+  </si>
+  <si>
+    <t>https://www.fontspace.com/dangernight-font-f86845</t>
+  </si>
+  <si>
+    <t>.button.rounded-large.rounded-gradient.large.icon-left</t>
+  </si>
+  <si>
+    <t>https://www.vidsplay.com/fall-foliage-aerial/</t>
+  </si>
+  <si>
+    <t>main-button.section--one__article__left__main-button</t>
+  </si>
+  <si>
+    <t>https://www.freedownloadmanager.org/</t>
+  </si>
+  <si>
+    <t>btn_text</t>
+  </si>
+  <si>
+    <t>https://wordpress.org/download/</t>
+  </si>
+  <si>
+    <t>wporg-modal__toggle wp-block-button__link</t>
+  </si>
+  <si>
+    <t>custom</t>
+  </si>
+  <si>
+    <t>https://www.neatdownloadmanager.com/index.php/en/</t>
+  </si>
+  <si>
+    <t>https://mattel163-limited-uno.en.uptodown.com/android/download</t>
+  </si>
+  <si>
+    <t>.button.download.active</t>
+  </si>
+  <si>
+    <t>btn-text</t>
+  </si>
+  <si>
+    <t>https://www.nvidia.com/en-eu/software/nvidia-app/</t>
+  </si>
+  <si>
+    <t>https://dotnet.microsoft.com/en-us/download</t>
+  </si>
+  <si>
+    <t>btn-magenta</t>
+  </si>
+  <si>
+    <t>https://www.webex.com/downloads.html</t>
+  </si>
+  <si>
+    <t>https://www.elastic.co/downloads/elasticsearch</t>
+  </si>
+  <si>
+    <t>button.icon-left.btn-primary.icon</t>
+  </si>
+  <si>
+    <t>https://www.postman.com/downloads/</t>
+  </si>
+  <si>
+    <t>.BaseButtonStyles-sc-18tp7ed-0.BaseButtonStyles__Primary-sc-18tp7ed-1.hSAEqA.hjMGj.mx-auto.w-100.mb-4</t>
+  </si>
+  <si>
+    <t>cmp-button</t>
+  </si>
+  <si>
+    <t>https://www.teamviewer.com/en-mea/download/windows/</t>
+  </si>
+  <si>
+    <t>https://www.viber.com/en/download/</t>
+  </si>
+  <si>
+    <t>global-btn</t>
   </si>
 </sst>
 </file>
@@ -14199,8 +14310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50E72B0-2073-4444-9809-60DAAE64F1E8}">
   <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B147" sqref="B147"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -14228,18 +14339,18 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="D4" s="19"/>
     </row>
@@ -14261,7 +14372,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>1505</v>
+        <v>1656</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>1504</v>
@@ -14269,54 +14380,62 @@
       <c r="H7" s="27"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
-      <c r="C8" s="33" t="s">
-        <v>19</v>
+      <c r="B8" s="21" t="s">
+        <v>1657</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>1658</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
-      <c r="C9" s="34" t="s">
-        <v>20</v>
+      <c r="B9" s="21" t="s">
+        <v>1654</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>1655</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="33" t="s">
-        <v>22</v>
+      <c r="B11" s="21" t="s">
+        <v>1660</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>1659</v>
       </c>
       <c r="H11" s="25"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
       <c r="C12" s="34" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="E12" s="26"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="C13" s="32" t="s">
-        <v>24</v>
+      <c r="B13" s="21" t="s">
+        <v>1662</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>1661</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -14326,9 +14445,11 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="33" t="s">
-        <v>27</v>
+      <c r="B16" s="21" t="s">
+        <v>1664</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>1663</v>
       </c>
       <c r="G16" s="26"/>
     </row>
@@ -14340,15 +14461,15 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="21" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>30</v>
@@ -14368,18 +14489,18 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="18" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C22" s="35" t="s">
         <v>1517</v>
-      </c>
-      <c r="C22" s="35" t="s">
-        <v>1518</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -14390,7 +14511,7 @@
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="21" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="C25" s="30" t="s">
         <v>36</v>
@@ -14418,18 +14539,18 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="21" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C30" s="36" t="s">
         <v>1522</v>
-      </c>
-      <c r="C30" s="36" t="s">
-        <v>1523</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="21" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -14452,7 +14573,7 @@
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="21" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="C35" s="35" t="s">
         <v>46</v>
@@ -14467,51 +14588,55 @@
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="21"/>
       <c r="C37" s="30" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="21" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
-        <v>1530</v>
-      </c>
-      <c r="C39" s="35" t="s">
-        <v>1531</v>
+        <v>1529</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>1653</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="21"/>
-      <c r="C40" s="33" t="s">
-        <v>51</v>
+      <c r="B40" s="21" t="s">
+        <v>1665</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>1666</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="21" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="21"/>
-      <c r="C43" s="33" t="s">
-        <v>54</v>
+      <c r="B43" s="21" t="s">
+        <v>1667</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>1668</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
@@ -14522,50 +14647,50 @@
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="21" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="C46" s="36" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="21" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="21" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="C48" s="36" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="21" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
       <c r="C49" s="30" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="21" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
@@ -14576,16 +14701,18 @@
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="21" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="C52" s="30" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="21"/>
-      <c r="C53" s="33" t="s">
-        <v>65</v>
+      <c r="B53" s="21" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>1671</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
@@ -14596,18 +14723,18 @@
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="21" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="C55" s="36" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="21" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
@@ -14618,16 +14745,16 @@
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="21" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="C58" s="36" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="21"/>
       <c r="C59" s="38" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
@@ -14649,25 +14776,27 @@
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="21"/>
-      <c r="C63" s="33" t="s">
-        <v>75</v>
+      <c r="B63" s="21" t="s">
+        <v>1674</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>1673</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="21" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="C64" s="30" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="21" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="C65" s="36" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
@@ -14678,10 +14807,10 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
@@ -14692,24 +14821,26 @@
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="21" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="C69" s="30" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="21"/>
-      <c r="C70" s="33" t="s">
-        <v>82</v>
+      <c r="B70" s="21" t="s">
+        <v>1508</v>
+      </c>
+      <c r="C70" s="30" t="s">
+        <v>1687</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="21" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
@@ -14719,17 +14850,19 @@
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="21"/>
-      <c r="C73" s="33" t="s">
-        <v>85</v>
+      <c r="B73" s="21" t="s">
+        <v>1676</v>
+      </c>
+      <c r="C73" s="30" t="s">
+        <v>1675</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="21" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="C74" s="30" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
@@ -14740,40 +14873,42 @@
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="21" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="C76" s="30" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="21" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="C77" s="34" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="21" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="C78" s="37" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="21" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="C79" s="39" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="21"/>
-      <c r="C80" s="33" t="s">
-        <v>92</v>
+      <c r="B80" s="21" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C80" s="30" t="s">
+        <v>1688</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
@@ -14784,18 +14919,18 @@
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="21" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="C82" s="30" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="21" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="C83" s="32" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
@@ -14805,15 +14940,19 @@
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" s="21"/>
-      <c r="C85" s="33" t="s">
-        <v>97</v>
+      <c r="B85" s="21" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C85" s="30" t="s">
+        <v>1677</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="21"/>
-      <c r="C86" s="33" t="s">
-        <v>98</v>
+      <c r="B86" s="21" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C86" s="34" t="s">
+        <v>1690</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
@@ -14824,10 +14963,10 @@
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="21" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="C88" s="30" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
@@ -14856,38 +14995,42 @@
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="21" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="C93" s="39" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="21" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="C94" s="37" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="21"/>
-      <c r="C95" s="33" t="s">
-        <v>107</v>
+      <c r="B95" s="21" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C95" s="34" t="s">
+        <v>1693</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="21" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="C96" s="30" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="21"/>
-      <c r="C97" s="33" t="s">
-        <v>109</v>
+      <c r="B97" s="21" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C97" s="30" t="s">
+        <v>1694</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
@@ -14922,34 +15065,34 @@
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="21" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="C103" s="30" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="21" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="C104" s="37" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="21" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="C105" s="39" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
       <c r="C106" s="37" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
@@ -14959,37 +15102,41 @@
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="21"/>
-      <c r="C108" s="33" t="s">
-        <v>120</v>
+      <c r="B108" s="21" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C108" s="32" t="s">
+        <v>1680</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="21"/>
       <c r="C109" s="39" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B110" s="21"/>
-      <c r="C110" s="33" t="s">
-        <v>1597</v>
+      <c r="B110" s="21" t="s">
+        <v>1682</v>
+      </c>
+      <c r="C110" s="37" t="s">
+        <v>1681</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="21" t="s">
-        <v>1598</v>
+        <v>1595</v>
       </c>
       <c r="C111" s="30" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="21" t="s">
-        <v>1600</v>
+        <v>1597</v>
       </c>
       <c r="C112" s="30" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
@@ -14999,253 +15146,259 @@
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B114" s="21"/>
-      <c r="C114" s="40" t="s">
-        <v>1604</v>
+      <c r="B114" s="21" t="s">
+        <v>1686</v>
+      </c>
+      <c r="C114" s="30" t="s">
+        <v>1685</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="21" t="s">
-        <v>1602</v>
-      </c>
-      <c r="C115" s="39" t="s">
-        <v>1603</v>
+        <v>1651</v>
+      </c>
+      <c r="C115" s="30" t="s">
+        <v>1652</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="21" t="s">
-        <v>1606</v>
+        <v>1600</v>
       </c>
       <c r="C116" s="30" t="s">
-        <v>1605</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="21" t="s">
-        <v>1608</v>
+        <v>1602</v>
       </c>
       <c r="C117" s="30" t="s">
-        <v>1607</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="21"/>
       <c r="C118" s="33" t="s">
-        <v>1609</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="21"/>
       <c r="C119" s="38" t="s">
-        <v>1610</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B120" s="21"/>
-      <c r="C120" s="40" t="s">
-        <v>1611</v>
+      <c r="B120" s="21" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C120" s="30" t="s">
+        <v>1669</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="21"/>
       <c r="C121" s="40" t="s">
-        <v>1612</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="21"/>
       <c r="C122" s="40" t="s">
-        <v>1613</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" s="21" t="s">
-        <v>1614</v>
+        <v>1607</v>
       </c>
       <c r="C123" s="30" t="s">
-        <v>1615</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" s="21" t="s">
-        <v>1616</v>
+        <v>1609</v>
       </c>
       <c r="C124" s="37" t="s">
-        <v>1617</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" s="21"/>
       <c r="C125" s="38" t="s">
-        <v>1618</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" s="21"/>
       <c r="C126" s="38" t="s">
-        <v>1619</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" s="21" t="s">
-        <v>1620</v>
+        <v>1613</v>
       </c>
       <c r="C127" s="39" t="s">
-        <v>1621</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" s="21" t="s">
-        <v>1622</v>
+        <v>1615</v>
       </c>
       <c r="C128" s="30" t="s">
-        <v>1623</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" s="21" t="s">
-        <v>1625</v>
+        <v>1618</v>
       </c>
       <c r="C129" s="30" t="s">
-        <v>1624</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="21"/>
       <c r="C130" s="38" t="s">
-        <v>1626</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="21"/>
       <c r="C131" s="38" t="s">
-        <v>1627</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="21"/>
       <c r="C132" s="38" t="s">
-        <v>1628</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="21"/>
       <c r="C133" s="38" t="s">
-        <v>1641</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="21"/>
       <c r="C134" s="38" t="s">
-        <v>1629</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="21"/>
       <c r="C135" s="38" t="s">
-        <v>1642</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="21" t="s">
-        <v>1630</v>
+        <v>1623</v>
       </c>
       <c r="C136" s="37" t="s">
-        <v>1631</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" s="21" t="s">
-        <v>1632</v>
+        <v>1625</v>
       </c>
       <c r="C137" s="37" t="s">
-        <v>1633</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="21"/>
       <c r="C138" s="39" t="s">
-        <v>1634</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="21"/>
       <c r="C139" s="38" t="s">
-        <v>1635</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" s="21" t="s">
-        <v>1636</v>
+        <v>1629</v>
       </c>
       <c r="C140" s="33" t="s">
-        <v>1637</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B141" s="21"/>
-      <c r="C141" s="40" t="s">
-        <v>1638</v>
+      <c r="B141" s="21" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C141" s="34" t="s">
+        <v>1684</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" s="21" t="s">
-        <v>1639</v>
+        <v>1631</v>
       </c>
       <c r="C142" s="30" t="s">
-        <v>1640</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="21" t="s">
-        <v>1644</v>
+        <v>1636</v>
       </c>
       <c r="C143" s="30" t="s">
-        <v>1643</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="21"/>
       <c r="C144" s="39" t="s">
-        <v>1645</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="21" t="s">
-        <v>1647</v>
+        <v>1639</v>
       </c>
       <c r="C145" s="30" t="s">
-        <v>1646</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" s="21" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="C146" s="30" t="s">
-        <v>1648</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" s="21" t="s">
-        <v>1650</v>
+        <v>1642</v>
       </c>
       <c r="C147" s="30" t="s">
-        <v>1649</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" s="21"/>
       <c r="C148" s="38" t="s">
-        <v>1651</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" s="21" t="s">
-        <v>1652</v>
+        <v>1644</v>
       </c>
       <c r="C149" s="32" t="s">
-        <v>1653</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
@@ -15262,177 +15415,177 @@
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" s="21" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C152" s="30" t="s">
-        <v>1656</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" s="21" t="s">
-        <v>1657</v>
+        <v>1649</v>
       </c>
       <c r="C153" s="32" t="s">
-        <v>1658</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" s="21" t="s">
-        <v>1655</v>
+        <v>1647</v>
       </c>
       <c r="C154" s="30" t="s">
-        <v>1654</v>
+        <v>1646</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1" xr:uid="{DF92E3AF-87D7-4B60-9BCE-C8679249E5F3}"/>
-    <hyperlink ref="C11" r:id="rId2" xr:uid="{DF0B2257-39B5-4A39-8727-C860512B1373}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{7DD31960-0368-4A27-9647-D08A1C574C38}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{E8018AD4-E1C3-4AAC-ADCD-179D91C5AB7B}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{574173E5-7719-43AD-B5BD-2043C15F8735}"/>
-    <hyperlink ref="C152" r:id="rId6" xr:uid="{68ECBF20-0D7B-437E-B689-4B068A1DB181}"/>
-    <hyperlink ref="C151" r:id="rId7" xr:uid="{16DA03B6-EC14-4CC2-907D-D5481694FAB8}"/>
-    <hyperlink ref="C10" r:id="rId8" xr:uid="{658462DC-D7E6-4931-A29E-C1A36593D1CB}"/>
-    <hyperlink ref="C150" r:id="rId9" xr:uid="{97C32394-AF94-4F0E-8A13-2FD594CD552E}"/>
-    <hyperlink ref="C9" r:id="rId10" xr:uid="{DD1E667C-49A1-43E2-9F3E-3A31DCE14D48}"/>
-    <hyperlink ref="C8" r:id="rId11" xr:uid="{3860EF84-5F21-4F8B-9DA0-1CB4E5991994}"/>
-    <hyperlink ref="C7" r:id="rId12" xr:uid="{9AF270F6-05FD-4ED2-BC8D-F08B5D664E41}"/>
-    <hyperlink ref="C6" r:id="rId13" xr:uid="{1BE1FD76-2B59-40AE-845C-447C6343496A}"/>
-    <hyperlink ref="C4" r:id="rId14" xr:uid="{2FC526BD-C17D-437A-89AD-2FE28D6023C2}"/>
-    <hyperlink ref="C13" r:id="rId15" xr:uid="{795EF266-492D-4C9F-A273-BD6048CB91FF}"/>
-    <hyperlink ref="C14" r:id="rId16" xr:uid="{B78E1107-D09B-41CD-9A06-AF7C646D7F34}"/>
-    <hyperlink ref="C15" r:id="rId17" xr:uid="{C9C027E3-C537-4F76-8B9F-FC7F498413E7}"/>
-    <hyperlink ref="C16" r:id="rId18" xr:uid="{BD32B382-FF07-4779-84A0-8BF88791EE61}"/>
-    <hyperlink ref="C17" r:id="rId19" xr:uid="{48ABC56C-60F8-4031-AE13-229847B91E92}"/>
-    <hyperlink ref="C18" r:id="rId20" xr:uid="{DB6A5354-22C6-40D5-9F50-9114BCFEF34E}"/>
-    <hyperlink ref="C19" r:id="rId21" xr:uid="{B5ABA31D-6FB7-4BA6-967E-923B838BEEA4}"/>
-    <hyperlink ref="C20" r:id="rId22" xr:uid="{6800F8E5-2104-4862-8630-2B6A1DE67597}"/>
-    <hyperlink ref="C21" r:id="rId23" xr:uid="{B5DA938E-D079-4252-94EE-937E3423F762}"/>
-    <hyperlink ref="C22" r:id="rId24" xr:uid="{8D647959-9418-4455-ACD2-918F5446F8B0}"/>
-    <hyperlink ref="C25" r:id="rId25" xr:uid="{0D35BE23-3125-44DF-AA15-BC9A13DAD4E0}"/>
-    <hyperlink ref="C23" r:id="rId26" xr:uid="{169E3BA7-6164-4A7F-9A88-84FF97BD02D6}"/>
-    <hyperlink ref="C24" r:id="rId27" xr:uid="{47D2533C-CE22-4504-A95C-D5DAC4A41415}"/>
-    <hyperlink ref="C27" r:id="rId28" xr:uid="{71F93FA1-617F-412E-9DFF-6E0D7405FB30}"/>
-    <hyperlink ref="C26" r:id="rId29" xr:uid="{064D4F68-8AE7-489F-A1CF-C7BFC9D2241D}"/>
-    <hyperlink ref="C28" r:id="rId30" xr:uid="{19B5E5DC-7AAC-4FCE-992A-E33AB214DA65}"/>
-    <hyperlink ref="C29" r:id="rId31" xr:uid="{350F50E6-C4D9-4F3A-B53D-144690D03D5A}"/>
-    <hyperlink ref="C30" r:id="rId32" location="google_vignette" xr:uid="{3754E26C-D7C6-40D3-B586-6975F6F56209}"/>
-    <hyperlink ref="C31" r:id="rId33" xr:uid="{537E3572-23A5-4B1C-94E7-1F64C6EB61B9}"/>
-    <hyperlink ref="C32" r:id="rId34" xr:uid="{B4520193-AB5F-40C5-9A4B-26529026A72E}"/>
-    <hyperlink ref="C33" r:id="rId35" xr:uid="{A9D65C0A-24AE-4D5B-BD49-0C336C536161}"/>
-    <hyperlink ref="C34" r:id="rId36" xr:uid="{18649552-0041-4234-A3EB-DFC8EC413712}"/>
-    <hyperlink ref="C35" r:id="rId37" xr:uid="{35032743-80F9-4C55-9D67-F35944398F85}"/>
-    <hyperlink ref="C36" r:id="rId38" xr:uid="{4F606619-1E1C-41D9-B617-DA116A1C0CA3}"/>
-    <hyperlink ref="C37" r:id="rId39" xr:uid="{B6F7B2EB-02A0-4D9E-A822-8BDA8286FC10}"/>
-    <hyperlink ref="C38" r:id="rId40" xr:uid="{74EB49E7-58BC-4E6C-B75B-265813B243D2}"/>
-    <hyperlink ref="C39" r:id="rId41" xr:uid="{4257C921-4F81-44E4-B6CA-183BE662305F}"/>
-    <hyperlink ref="C40" r:id="rId42" xr:uid="{A65B2ECB-F8D3-4FF6-8201-C7D0EBD6A9F1}"/>
-    <hyperlink ref="C41" r:id="rId43" xr:uid="{C8A70CAD-E2DA-4809-B1D1-2F662B3D0486}"/>
-    <hyperlink ref="C42" r:id="rId44" xr:uid="{2F69EF8D-C6D5-44FB-A957-5FAD77F891F0}"/>
-    <hyperlink ref="C43" r:id="rId45" xr:uid="{B9939436-D276-4A35-B3B5-8E625EBA6037}"/>
-    <hyperlink ref="C44" r:id="rId46" xr:uid="{E8D3DF2E-D6BC-47CA-AF40-8D1C537A5571}"/>
-    <hyperlink ref="C45" r:id="rId47" xr:uid="{5C1BD0FA-31B0-4F22-981A-667C6150C2E6}"/>
-    <hyperlink ref="C46" r:id="rId48" xr:uid="{814E9C6C-074D-4418-829E-E1F3359B338F}"/>
-    <hyperlink ref="C50" r:id="rId49" location="kali-installer-images" xr:uid="{E1BCFBC9-0B68-431D-90DA-0369C5382AD4}"/>
-    <hyperlink ref="C47" r:id="rId50" xr:uid="{EC716333-E69B-4EFE-BE63-E604B21F9EBF}"/>
-    <hyperlink ref="C48" r:id="rId51" xr:uid="{743525DA-D392-4530-8242-1F48B502FA4E}"/>
-    <hyperlink ref="C49" r:id="rId52" xr:uid="{A38A5E98-F896-46B4-8A2E-3E80D787816F}"/>
-    <hyperlink ref="C51" r:id="rId53" xr:uid="{823493CB-2620-4D09-AA8F-7A9857E24D01}"/>
-    <hyperlink ref="C53" r:id="rId54" xr:uid="{8183C350-9FC9-4B12-BAD5-4152FEE6040A}"/>
-    <hyperlink ref="C54" r:id="rId55" xr:uid="{8FDE9EF9-40DB-4296-9945-146497DF033A}"/>
-    <hyperlink ref="C55" r:id="rId56" xr:uid="{1E30EDA7-8A17-490D-89DD-F09092EF3230}"/>
-    <hyperlink ref="C56" r:id="rId57" xr:uid="{7D60A2E9-1459-4CC0-A3D8-3F8B6D24EDD7}"/>
-    <hyperlink ref="C57" r:id="rId58" xr:uid="{9FB30596-CDD4-47A8-AE6B-CAC81B53BAC0}"/>
-    <hyperlink ref="C58" r:id="rId59" xr:uid="{D0CFA84A-4EB8-4E3A-854E-9AFE4E3FDA16}"/>
-    <hyperlink ref="C64" r:id="rId60" xr:uid="{A9D99C97-92B1-4979-B86E-32BC99DCF5D6}"/>
-    <hyperlink ref="C65" r:id="rId61" xr:uid="{123E1AAE-E0F6-4625-8F67-8146F97BB4E1}"/>
-    <hyperlink ref="C67" r:id="rId62" xr:uid="{B91B8090-78B6-48FF-A863-E1651AB8D7CF}"/>
-    <hyperlink ref="C66" r:id="rId63" xr:uid="{7048EAAD-48CA-4B1B-A3F7-F4F1EA614A73}"/>
-    <hyperlink ref="C68" r:id="rId64" xr:uid="{354DCF7C-3DC5-4A83-A807-C4E207675DF1}"/>
-    <hyperlink ref="C69" r:id="rId65" xr:uid="{D3246893-3FB0-40DF-8B20-1686D9D450DA}"/>
-    <hyperlink ref="C70" r:id="rId66" xr:uid="{231A8279-B117-4F92-A2E2-F06FBB83AF2A}"/>
-    <hyperlink ref="C71" r:id="rId67" xr:uid="{5D2770CE-1672-4FDE-8D9E-6D86E70E88D7}"/>
-    <hyperlink ref="C72" r:id="rId68" xr:uid="{E9868362-8964-4567-ABDF-BE883ADB7549}"/>
-    <hyperlink ref="C73" r:id="rId69" xr:uid="{0ACB5CBE-8908-4471-A689-373CE8DEB745}"/>
-    <hyperlink ref="C74" r:id="rId70" xr:uid="{FD609230-2D31-4E2E-B524-87A25007B12F}"/>
-    <hyperlink ref="C75" r:id="rId71" xr:uid="{C0AE8560-BE27-415A-AD0A-14E3797E5B20}"/>
-    <hyperlink ref="C76" r:id="rId72" xr:uid="{4868C4DD-96B1-44D7-8B96-F9295A5A0DCD}"/>
-    <hyperlink ref="C77" r:id="rId73" xr:uid="{25E5301F-61E6-43D2-A641-2F6026FF1480}"/>
-    <hyperlink ref="C78" r:id="rId74" xr:uid="{CBE9D00B-0CC6-4D93-8C7E-9C10BAAC47EE}"/>
-    <hyperlink ref="C79" r:id="rId75" xr:uid="{4D5A2527-8BE9-4F08-9D4C-87D6491402AB}"/>
-    <hyperlink ref="C80" r:id="rId76" xr:uid="{28E2B9FC-AB8B-44C7-8B21-0E1E522F10F7}"/>
-    <hyperlink ref="C81" r:id="rId77" xr:uid="{FA281B91-D05B-4C2B-B507-034DB0460365}"/>
-    <hyperlink ref="C82" r:id="rId78" xr:uid="{89740D7E-60F5-4477-B0F5-482D59C91D1D}"/>
-    <hyperlink ref="C83" r:id="rId79" xr:uid="{2EE40B56-5EA1-421E-863D-EBB257790F35}"/>
-    <hyperlink ref="C59" r:id="rId80" xr:uid="{0D69ECB9-6D5C-431C-80C2-EAF05F31B7F4}"/>
-    <hyperlink ref="C84" r:id="rId81" xr:uid="{D95162B2-AB17-430D-A4AA-59E72D376090}"/>
-    <hyperlink ref="C85" r:id="rId82" xr:uid="{3A8F3135-C2E5-42BB-B039-BC7B4D4CEB46}"/>
-    <hyperlink ref="C86" r:id="rId83" xr:uid="{33811B59-87F3-45DD-9166-C307BAC98B35}"/>
-    <hyperlink ref="C87" r:id="rId84" xr:uid="{BB4F0EFA-A1E0-4AAA-91C7-8886F4840C66}"/>
-    <hyperlink ref="C88" r:id="rId85" xr:uid="{0F18BA5D-0A7A-442D-AD02-F2C623AEA04F}"/>
-    <hyperlink ref="C89" r:id="rId86" xr:uid="{77B195E5-961B-4E0C-989E-BCAB90FE6D5A}"/>
-    <hyperlink ref="C90" r:id="rId87" xr:uid="{B98A95F5-8F2A-4445-ABDC-34E189C133C5}"/>
-    <hyperlink ref="C91" r:id="rId88" xr:uid="{5D7D8938-B362-47C3-9537-12308E080143}"/>
-    <hyperlink ref="C92" r:id="rId89" xr:uid="{592DA57C-A13F-43E9-8B81-3AECF9B3E245}"/>
-    <hyperlink ref="C93" r:id="rId90" location="download" xr:uid="{6A65D0F3-344D-43BA-9B91-9B0E06D8E2E6}"/>
-    <hyperlink ref="C94" r:id="rId91" xr:uid="{79F56FA6-8F91-4B9F-8B40-ECB07CED87AE}"/>
-    <hyperlink ref="C95" r:id="rId92" xr:uid="{F8BC4287-42BB-4D7F-BCC2-C5970212A8B7}"/>
-    <hyperlink ref="C96" r:id="rId93" xr:uid="{7D5221D7-7E6A-4274-B4CE-B5E04F892D2F}"/>
-    <hyperlink ref="C97" r:id="rId94" xr:uid="{D8A46ABB-98D1-422B-AE92-E9295766C282}"/>
-    <hyperlink ref="C98" r:id="rId95" xr:uid="{48415821-BF59-45C0-B636-B15716A8AFBE}"/>
-    <hyperlink ref="C99" r:id="rId96" xr:uid="{3F881E20-3181-4372-B4E2-6B3AF72EB3A5}"/>
-    <hyperlink ref="C100" r:id="rId97" xr:uid="{0444AA34-7704-4F15-B46C-22C38E0B5309}"/>
-    <hyperlink ref="C101" r:id="rId98" xr:uid="{F87C2EA2-D052-4A96-AB0D-42085AF2F6EA}"/>
-    <hyperlink ref="C102" r:id="rId99" xr:uid="{7E914BAB-4F68-4D85-BC6B-92D5DE40739C}"/>
-    <hyperlink ref="C103" r:id="rId100" xr:uid="{9BDF66C9-25BE-449E-828E-2EC717720208}"/>
-    <hyperlink ref="C104" r:id="rId101" xr:uid="{D0E8F201-9C1A-4BF1-8DA2-95046CD31165}"/>
-    <hyperlink ref="C105" r:id="rId102" xr:uid="{DC34E626-90BC-4E82-AC86-B39CDA345EC2}"/>
-    <hyperlink ref="C106" r:id="rId103" xr:uid="{E430BC28-7E12-486D-B301-68AA34A492DD}"/>
-    <hyperlink ref="C107" r:id="rId104" xr:uid="{C3115C55-EC7B-45E3-8662-226D73A716DD}"/>
-    <hyperlink ref="C108" r:id="rId105" xr:uid="{16E59904-31C8-48FB-A058-33975EA173F1}"/>
-    <hyperlink ref="C109" r:id="rId106" location="/media/File:2019_City_of_London_3D_model.jpg" xr:uid="{D8008C1B-63BB-4DAB-ADCD-C3A71D666E7C}"/>
-    <hyperlink ref="C110" r:id="rId107" xr:uid="{D1CCBCC4-9A44-4453-98DE-989C25F78BC3}"/>
-    <hyperlink ref="C111" r:id="rId108" xr:uid="{7F0DA02A-2A72-4557-9412-46FB6F76C781}"/>
-    <hyperlink ref="C112" r:id="rId109" xr:uid="{53A4E879-856F-436F-A8DC-3257683B02B1}"/>
-    <hyperlink ref="C115" r:id="rId110" xr:uid="{9F0C7A20-F85A-4FB3-B05E-58FBD30122EE}"/>
-    <hyperlink ref="C113" r:id="rId111" xr:uid="{4F49A94A-FCA6-46DC-B727-A9BEBBD65D84}"/>
-    <hyperlink ref="C114" r:id="rId112" xr:uid="{205D2E03-E232-42E5-B438-A6BC4AF79C03}"/>
-    <hyperlink ref="C116" r:id="rId113" location="fromView=keyword&amp;page=1&amp;position=2&amp;uuid=f2d9c8ff-4958-4fdf-a220-d39d4c853740&amp;from_element=categories_trends&amp;query=University+Teacher" display="https://www.freepik.com/free-photo/young-woman-teacher-wearing-glasses-explaining-lesson-holding-stack-books-looking-confident-standing-school-desk-front-blackboard-classroom_26397314.htm#fromView=keyword&amp;page=1&amp;position=2&amp;uuid=f2d9c8ff-4958-4fdf-a220-d39d4c853740&amp;from_element=categories_trends&amp;query=University+Teacher" xr:uid="{63CB67EA-23F9-45B4-9DC7-8FD2FB007797}"/>
-    <hyperlink ref="C117" r:id="rId114" xr:uid="{A52B4FAE-450E-4385-B259-61D9DDBF9587}"/>
-    <hyperlink ref="C118" r:id="rId115" xr:uid="{4879ACB0-AB3E-4858-9477-768BD1BC3B6F}"/>
-    <hyperlink ref="C153" r:id="rId116" xr:uid="{27F4667C-E73F-4D70-A01A-4C4795729965}"/>
-    <hyperlink ref="C119" r:id="rId117" xr:uid="{4A8F39D5-A16F-4A0B-8166-BB7AE8B590F1}"/>
-    <hyperlink ref="C120" r:id="rId118" xr:uid="{E729AAFB-923C-4752-9548-677B4A0CBCB1}"/>
-    <hyperlink ref="C121" r:id="rId119" xr:uid="{8602DFAA-7B01-4481-AA3B-F6EAE34449C9}"/>
-    <hyperlink ref="C122" r:id="rId120" xr:uid="{8EEDA427-C69D-4C39-8F43-58262A593AFE}"/>
-    <hyperlink ref="C123" r:id="rId121" xr:uid="{AB39E989-5BE0-483C-9750-97DBF6733693}"/>
-    <hyperlink ref="C124" r:id="rId122" xr:uid="{75694668-2FF0-43B0-BFF3-1F2C90B9B74A}"/>
-    <hyperlink ref="C125" r:id="rId123" xr:uid="{A5202F31-89AE-4187-BD14-11BC381A35E0}"/>
-    <hyperlink ref="C126" r:id="rId124" xr:uid="{BD8F8097-6FDD-48AF-8E0E-63FBF4EAEF19}"/>
-    <hyperlink ref="C127" r:id="rId125" xr:uid="{ABE75258-5BF6-44E1-8CA4-305E9FD2216F}"/>
-    <hyperlink ref="C128" r:id="rId126" location="google_vignette" xr:uid="{2A87507C-829A-410D-B0C6-309D4E3A2BD3}"/>
-    <hyperlink ref="C129" r:id="rId127" xr:uid="{625B0886-C44A-4063-8A39-4883D1980498}"/>
-    <hyperlink ref="C130" r:id="rId128" xr:uid="{CEE57B0B-A828-4DD4-83A8-A9C38D9D8DBE}"/>
-    <hyperlink ref="C131" r:id="rId129" xr:uid="{ADB11BDE-27E8-423F-AFDB-5FAAA3892804}"/>
-    <hyperlink ref="C132" r:id="rId130" xr:uid="{DE3934B6-FED0-4609-A6E0-986ABAC1CE69}"/>
-    <hyperlink ref="C134" r:id="rId131" xr:uid="{4156FCA5-20E1-4801-A3EB-FB1100E2354A}"/>
-    <hyperlink ref="C136" r:id="rId132" xr:uid="{1B83D7CB-D69B-498C-9CAC-4BB8F195C9F4}"/>
-    <hyperlink ref="C137" r:id="rId133" xr:uid="{ED7E2358-B5A9-4DA1-89AC-42221E44451D}"/>
-    <hyperlink ref="C138" r:id="rId134" xr:uid="{00B2CF8C-A349-46F9-99D0-73A40EAC8BCD}"/>
-    <hyperlink ref="C139" r:id="rId135" xr:uid="{0168C140-1EBD-4635-A27B-A1F6DB707B99}"/>
-    <hyperlink ref="C140" r:id="rId136" xr:uid="{32E59C3E-FA98-4923-8EE6-5E998F112CE1}"/>
-    <hyperlink ref="C141" r:id="rId137" xr:uid="{98D84775-7F44-47A9-BD91-2984B1DD5E7A}"/>
-    <hyperlink ref="C142" r:id="rId138" xr:uid="{50CF528A-B2AD-4844-863A-ED656E183E4D}"/>
-    <hyperlink ref="C133" r:id="rId139" xr:uid="{F6802C6B-31C7-43A4-9758-44BBE446B47A}"/>
-    <hyperlink ref="C135" r:id="rId140" xr:uid="{0E7140E4-72ED-43C7-9ACB-E28E8B6AEBA4}"/>
-    <hyperlink ref="C143" r:id="rId141" xr:uid="{B58922D1-EFBD-4E0F-B032-F3D207B54A16}"/>
-    <hyperlink ref="C145" r:id="rId142" xr:uid="{25F446AC-A40C-4543-890F-2EFC06F6FC1E}"/>
-    <hyperlink ref="C146" r:id="rId143" xr:uid="{3B322F6E-7E7F-4DE7-95E7-C3DBF7ABB633}"/>
-    <hyperlink ref="C147" r:id="rId144" xr:uid="{3ED732A0-1BE2-420B-93EC-8C04838DC24D}"/>
-    <hyperlink ref="C148" r:id="rId145" xr:uid="{6E223FF5-B6CD-4E57-8DBA-4F47D5A4544F}"/>
-    <hyperlink ref="C149" r:id="rId146" xr:uid="{8BA115F0-9A73-4E7E-8C04-39FF7AABC875}"/>
-    <hyperlink ref="C154" r:id="rId147" xr:uid="{C8852A29-E984-41D6-865B-C7F453D536FB}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{7DD31960-0368-4A27-9647-D08A1C574C38}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{E8018AD4-E1C3-4AAC-ADCD-179D91C5AB7B}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{574173E5-7719-43AD-B5BD-2043C15F8735}"/>
+    <hyperlink ref="C152" r:id="rId5" xr:uid="{68ECBF20-0D7B-437E-B689-4B068A1DB181}"/>
+    <hyperlink ref="C151" r:id="rId6" xr:uid="{16DA03B6-EC14-4CC2-907D-D5481694FAB8}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{658462DC-D7E6-4931-A29E-C1A36593D1CB}"/>
+    <hyperlink ref="C150" r:id="rId8" xr:uid="{97C32394-AF94-4F0E-8A13-2FD594CD552E}"/>
+    <hyperlink ref="C9" r:id="rId9" xr:uid="{DD1E667C-49A1-43E2-9F3E-3A31DCE14D48}"/>
+    <hyperlink ref="C7" r:id="rId10" xr:uid="{9AF270F6-05FD-4ED2-BC8D-F08B5D664E41}"/>
+    <hyperlink ref="C6" r:id="rId11" xr:uid="{1BE1FD76-2B59-40AE-845C-447C6343496A}"/>
+    <hyperlink ref="C4" r:id="rId12" xr:uid="{2FC526BD-C17D-437A-89AD-2FE28D6023C2}"/>
+    <hyperlink ref="C13" r:id="rId13" xr:uid="{795EF266-492D-4C9F-A273-BD6048CB91FF}"/>
+    <hyperlink ref="C14" r:id="rId14" xr:uid="{B78E1107-D09B-41CD-9A06-AF7C646D7F34}"/>
+    <hyperlink ref="C15" r:id="rId15" xr:uid="{C9C027E3-C537-4F76-8B9F-FC7F498413E7}"/>
+    <hyperlink ref="C16" r:id="rId16" xr:uid="{BD32B382-FF07-4779-84A0-8BF88791EE61}"/>
+    <hyperlink ref="C17" r:id="rId17" xr:uid="{48ABC56C-60F8-4031-AE13-229847B91E92}"/>
+    <hyperlink ref="C18" r:id="rId18" xr:uid="{DB6A5354-22C6-40D5-9F50-9114BCFEF34E}"/>
+    <hyperlink ref="C19" r:id="rId19" xr:uid="{B5ABA31D-6FB7-4BA6-967E-923B838BEEA4}"/>
+    <hyperlink ref="C20" r:id="rId20" xr:uid="{6800F8E5-2104-4862-8630-2B6A1DE67597}"/>
+    <hyperlink ref="C21" r:id="rId21" xr:uid="{B5DA938E-D079-4252-94EE-937E3423F762}"/>
+    <hyperlink ref="C22" r:id="rId22" xr:uid="{8D647959-9418-4455-ACD2-918F5446F8B0}"/>
+    <hyperlink ref="C25" r:id="rId23" xr:uid="{0D35BE23-3125-44DF-AA15-BC9A13DAD4E0}"/>
+    <hyperlink ref="C23" r:id="rId24" xr:uid="{169E3BA7-6164-4A7F-9A88-84FF97BD02D6}"/>
+    <hyperlink ref="C24" r:id="rId25" xr:uid="{47D2533C-CE22-4504-A95C-D5DAC4A41415}"/>
+    <hyperlink ref="C27" r:id="rId26" xr:uid="{71F93FA1-617F-412E-9DFF-6E0D7405FB30}"/>
+    <hyperlink ref="C26" r:id="rId27" xr:uid="{064D4F68-8AE7-489F-A1CF-C7BFC9D2241D}"/>
+    <hyperlink ref="C28" r:id="rId28" xr:uid="{19B5E5DC-7AAC-4FCE-992A-E33AB214DA65}"/>
+    <hyperlink ref="C29" r:id="rId29" xr:uid="{350F50E6-C4D9-4F3A-B53D-144690D03D5A}"/>
+    <hyperlink ref="C30" r:id="rId30" location="google_vignette" xr:uid="{3754E26C-D7C6-40D3-B586-6975F6F56209}"/>
+    <hyperlink ref="C31" r:id="rId31" xr:uid="{537E3572-23A5-4B1C-94E7-1F64C6EB61B9}"/>
+    <hyperlink ref="C32" r:id="rId32" xr:uid="{B4520193-AB5F-40C5-9A4B-26529026A72E}"/>
+    <hyperlink ref="C33" r:id="rId33" xr:uid="{A9D65C0A-24AE-4D5B-BD49-0C336C536161}"/>
+    <hyperlink ref="C34" r:id="rId34" xr:uid="{18649552-0041-4234-A3EB-DFC8EC413712}"/>
+    <hyperlink ref="C35" r:id="rId35" xr:uid="{35032743-80F9-4C55-9D67-F35944398F85}"/>
+    <hyperlink ref="C36" r:id="rId36" xr:uid="{4F606619-1E1C-41D9-B617-DA116A1C0CA3}"/>
+    <hyperlink ref="C37" r:id="rId37" xr:uid="{B6F7B2EB-02A0-4D9E-A822-8BDA8286FC10}"/>
+    <hyperlink ref="C38" r:id="rId38" xr:uid="{74EB49E7-58BC-4E6C-B75B-265813B243D2}"/>
+    <hyperlink ref="C39" r:id="rId39" xr:uid="{4257C921-4F81-44E4-B6CA-183BE662305F}"/>
+    <hyperlink ref="C40" r:id="rId40" xr:uid="{A65B2ECB-F8D3-4FF6-8201-C7D0EBD6A9F1}"/>
+    <hyperlink ref="C41" r:id="rId41" xr:uid="{C8A70CAD-E2DA-4809-B1D1-2F662B3D0486}"/>
+    <hyperlink ref="C42" r:id="rId42" xr:uid="{2F69EF8D-C6D5-44FB-A957-5FAD77F891F0}"/>
+    <hyperlink ref="C43" r:id="rId43" xr:uid="{B9939436-D276-4A35-B3B5-8E625EBA6037}"/>
+    <hyperlink ref="C44" r:id="rId44" xr:uid="{E8D3DF2E-D6BC-47CA-AF40-8D1C537A5571}"/>
+    <hyperlink ref="C45" r:id="rId45" xr:uid="{5C1BD0FA-31B0-4F22-981A-667C6150C2E6}"/>
+    <hyperlink ref="C46" r:id="rId46" xr:uid="{814E9C6C-074D-4418-829E-E1F3359B338F}"/>
+    <hyperlink ref="C50" r:id="rId47" location="kali-installer-images" xr:uid="{E1BCFBC9-0B68-431D-90DA-0369C5382AD4}"/>
+    <hyperlink ref="C47" r:id="rId48" xr:uid="{EC716333-E69B-4EFE-BE63-E604B21F9EBF}"/>
+    <hyperlink ref="C48" r:id="rId49" xr:uid="{743525DA-D392-4530-8242-1F48B502FA4E}"/>
+    <hyperlink ref="C49" r:id="rId50" xr:uid="{A38A5E98-F896-46B4-8A2E-3E80D787816F}"/>
+    <hyperlink ref="C51" r:id="rId51" xr:uid="{823493CB-2620-4D09-AA8F-7A9857E24D01}"/>
+    <hyperlink ref="C54" r:id="rId52" xr:uid="{8FDE9EF9-40DB-4296-9945-146497DF033A}"/>
+    <hyperlink ref="C55" r:id="rId53" xr:uid="{1E30EDA7-8A17-490D-89DD-F09092EF3230}"/>
+    <hyperlink ref="C56" r:id="rId54" xr:uid="{7D60A2E9-1459-4CC0-A3D8-3F8B6D24EDD7}"/>
+    <hyperlink ref="C57" r:id="rId55" xr:uid="{9FB30596-CDD4-47A8-AE6B-CAC81B53BAC0}"/>
+    <hyperlink ref="C58" r:id="rId56" xr:uid="{D0CFA84A-4EB8-4E3A-854E-9AFE4E3FDA16}"/>
+    <hyperlink ref="C64" r:id="rId57" xr:uid="{A9D99C97-92B1-4979-B86E-32BC99DCF5D6}"/>
+    <hyperlink ref="C65" r:id="rId58" xr:uid="{123E1AAE-E0F6-4625-8F67-8146F97BB4E1}"/>
+    <hyperlink ref="C67" r:id="rId59" xr:uid="{B91B8090-78B6-48FF-A863-E1651AB8D7CF}"/>
+    <hyperlink ref="C66" r:id="rId60" xr:uid="{7048EAAD-48CA-4B1B-A3F7-F4F1EA614A73}"/>
+    <hyperlink ref="C68" r:id="rId61" xr:uid="{354DCF7C-3DC5-4A83-A807-C4E207675DF1}"/>
+    <hyperlink ref="C69" r:id="rId62" xr:uid="{D3246893-3FB0-40DF-8B20-1686D9D450DA}"/>
+    <hyperlink ref="C71" r:id="rId63" xr:uid="{5D2770CE-1672-4FDE-8D9E-6D86E70E88D7}"/>
+    <hyperlink ref="C72" r:id="rId64" xr:uid="{E9868362-8964-4567-ABDF-BE883ADB7549}"/>
+    <hyperlink ref="C73" r:id="rId65" xr:uid="{0ACB5CBE-8908-4471-A689-373CE8DEB745}"/>
+    <hyperlink ref="C74" r:id="rId66" xr:uid="{FD609230-2D31-4E2E-B524-87A25007B12F}"/>
+    <hyperlink ref="C75" r:id="rId67" xr:uid="{C0AE8560-BE27-415A-AD0A-14E3797E5B20}"/>
+    <hyperlink ref="C76" r:id="rId68" xr:uid="{4868C4DD-96B1-44D7-8B96-F9295A5A0DCD}"/>
+    <hyperlink ref="C77" r:id="rId69" xr:uid="{25E5301F-61E6-43D2-A641-2F6026FF1480}"/>
+    <hyperlink ref="C78" r:id="rId70" xr:uid="{CBE9D00B-0CC6-4D93-8C7E-9C10BAAC47EE}"/>
+    <hyperlink ref="C79" r:id="rId71" xr:uid="{4D5A2527-8BE9-4F08-9D4C-87D6491402AB}"/>
+    <hyperlink ref="C80" r:id="rId72" xr:uid="{28E2B9FC-AB8B-44C7-8B21-0E1E522F10F7}"/>
+    <hyperlink ref="C81" r:id="rId73" xr:uid="{FA281B91-D05B-4C2B-B507-034DB0460365}"/>
+    <hyperlink ref="C82" r:id="rId74" xr:uid="{89740D7E-60F5-4477-B0F5-482D59C91D1D}"/>
+    <hyperlink ref="C83" r:id="rId75" xr:uid="{2EE40B56-5EA1-421E-863D-EBB257790F35}"/>
+    <hyperlink ref="C59" r:id="rId76" xr:uid="{0D69ECB9-6D5C-431C-80C2-EAF05F31B7F4}"/>
+    <hyperlink ref="C84" r:id="rId77" xr:uid="{D95162B2-AB17-430D-A4AA-59E72D376090}"/>
+    <hyperlink ref="C85" r:id="rId78" xr:uid="{3A8F3135-C2E5-42BB-B039-BC7B4D4CEB46}"/>
+    <hyperlink ref="C86" r:id="rId79" xr:uid="{33811B59-87F3-45DD-9166-C307BAC98B35}"/>
+    <hyperlink ref="C87" r:id="rId80" xr:uid="{BB4F0EFA-A1E0-4AAA-91C7-8886F4840C66}"/>
+    <hyperlink ref="C88" r:id="rId81" xr:uid="{0F18BA5D-0A7A-442D-AD02-F2C623AEA04F}"/>
+    <hyperlink ref="C89" r:id="rId82" xr:uid="{77B195E5-961B-4E0C-989E-BCAB90FE6D5A}"/>
+    <hyperlink ref="C90" r:id="rId83" xr:uid="{B98A95F5-8F2A-4445-ABDC-34E189C133C5}"/>
+    <hyperlink ref="C91" r:id="rId84" xr:uid="{5D7D8938-B362-47C3-9537-12308E080143}"/>
+    <hyperlink ref="C92" r:id="rId85" xr:uid="{592DA57C-A13F-43E9-8B81-3AECF9B3E245}"/>
+    <hyperlink ref="C93" r:id="rId86" location="download" xr:uid="{6A65D0F3-344D-43BA-9B91-9B0E06D8E2E6}"/>
+    <hyperlink ref="C94" r:id="rId87" xr:uid="{79F56FA6-8F91-4B9F-8B40-ECB07CED87AE}"/>
+    <hyperlink ref="C95" r:id="rId88" xr:uid="{F8BC4287-42BB-4D7F-BCC2-C5970212A8B7}"/>
+    <hyperlink ref="C96" r:id="rId89" xr:uid="{7D5221D7-7E6A-4274-B4CE-B5E04F892D2F}"/>
+    <hyperlink ref="C97" r:id="rId90" xr:uid="{D8A46ABB-98D1-422B-AE92-E9295766C282}"/>
+    <hyperlink ref="C98" r:id="rId91" xr:uid="{48415821-BF59-45C0-B636-B15716A8AFBE}"/>
+    <hyperlink ref="C99" r:id="rId92" xr:uid="{3F881E20-3181-4372-B4E2-6B3AF72EB3A5}"/>
+    <hyperlink ref="C100" r:id="rId93" xr:uid="{0444AA34-7704-4F15-B46C-22C38E0B5309}"/>
+    <hyperlink ref="C101" r:id="rId94" xr:uid="{F87C2EA2-D052-4A96-AB0D-42085AF2F6EA}"/>
+    <hyperlink ref="C102" r:id="rId95" xr:uid="{7E914BAB-4F68-4D85-BC6B-92D5DE40739C}"/>
+    <hyperlink ref="C103" r:id="rId96" xr:uid="{9BDF66C9-25BE-449E-828E-2EC717720208}"/>
+    <hyperlink ref="C104" r:id="rId97" xr:uid="{D0E8F201-9C1A-4BF1-8DA2-95046CD31165}"/>
+    <hyperlink ref="C105" r:id="rId98" xr:uid="{DC34E626-90BC-4E82-AC86-B39CDA345EC2}"/>
+    <hyperlink ref="C106" r:id="rId99" xr:uid="{E430BC28-7E12-486D-B301-68AA34A492DD}"/>
+    <hyperlink ref="C107" r:id="rId100" xr:uid="{C3115C55-EC7B-45E3-8662-226D73A716DD}"/>
+    <hyperlink ref="C108" r:id="rId101" xr:uid="{16E59904-31C8-48FB-A058-33975EA173F1}"/>
+    <hyperlink ref="C109" r:id="rId102" location="/media/File:2019_City_of_London_3D_model.jpg" xr:uid="{D8008C1B-63BB-4DAB-ADCD-C3A71D666E7C}"/>
+    <hyperlink ref="C110" r:id="rId103" xr:uid="{D1CCBCC4-9A44-4453-98DE-989C25F78BC3}"/>
+    <hyperlink ref="C111" r:id="rId104" xr:uid="{7F0DA02A-2A72-4557-9412-46FB6F76C781}"/>
+    <hyperlink ref="C112" r:id="rId105" xr:uid="{53A4E879-856F-436F-A8DC-3257683B02B1}"/>
+    <hyperlink ref="C115" r:id="rId106" xr:uid="{9F0C7A20-F85A-4FB3-B05E-58FBD30122EE}"/>
+    <hyperlink ref="C113" r:id="rId107" xr:uid="{4F49A94A-FCA6-46DC-B727-A9BEBBD65D84}"/>
+    <hyperlink ref="C116" r:id="rId108" location="fromView=keyword&amp;page=1&amp;position=2&amp;uuid=f2d9c8ff-4958-4fdf-a220-d39d4c853740&amp;from_element=categories_trends&amp;query=University+Teacher" display="https://www.freepik.com/free-photo/young-woman-teacher-wearing-glasses-explaining-lesson-holding-stack-books-looking-confident-standing-school-desk-front-blackboard-classroom_26397314.htm#fromView=keyword&amp;page=1&amp;position=2&amp;uuid=f2d9c8ff-4958-4fdf-a220-d39d4c853740&amp;from_element=categories_trends&amp;query=University+Teacher" xr:uid="{63CB67EA-23F9-45B4-9DC7-8FD2FB007797}"/>
+    <hyperlink ref="C117" r:id="rId109" xr:uid="{A52B4FAE-450E-4385-B259-61D9DDBF9587}"/>
+    <hyperlink ref="C118" r:id="rId110" xr:uid="{4879ACB0-AB3E-4858-9477-768BD1BC3B6F}"/>
+    <hyperlink ref="C153" r:id="rId111" xr:uid="{27F4667C-E73F-4D70-A01A-4C4795729965}"/>
+    <hyperlink ref="C119" r:id="rId112" xr:uid="{4A8F39D5-A16F-4A0B-8166-BB7AE8B590F1}"/>
+    <hyperlink ref="C120" r:id="rId113" xr:uid="{E729AAFB-923C-4752-9548-677B4A0CBCB1}"/>
+    <hyperlink ref="C121" r:id="rId114" xr:uid="{8602DFAA-7B01-4481-AA3B-F6EAE34449C9}"/>
+    <hyperlink ref="C122" r:id="rId115" xr:uid="{8EEDA427-C69D-4C39-8F43-58262A593AFE}"/>
+    <hyperlink ref="C123" r:id="rId116" xr:uid="{AB39E989-5BE0-483C-9750-97DBF6733693}"/>
+    <hyperlink ref="C124" r:id="rId117" xr:uid="{75694668-2FF0-43B0-BFF3-1F2C90B9B74A}"/>
+    <hyperlink ref="C125" r:id="rId118" xr:uid="{A5202F31-89AE-4187-BD14-11BC381A35E0}"/>
+    <hyperlink ref="C126" r:id="rId119" xr:uid="{BD8F8097-6FDD-48AF-8E0E-63FBF4EAEF19}"/>
+    <hyperlink ref="C127" r:id="rId120" xr:uid="{ABE75258-5BF6-44E1-8CA4-305E9FD2216F}"/>
+    <hyperlink ref="C128" r:id="rId121" location="google_vignette" xr:uid="{2A87507C-829A-410D-B0C6-309D4E3A2BD3}"/>
+    <hyperlink ref="C129" r:id="rId122" xr:uid="{625B0886-C44A-4063-8A39-4883D1980498}"/>
+    <hyperlink ref="C130" r:id="rId123" xr:uid="{CEE57B0B-A828-4DD4-83A8-A9C38D9D8DBE}"/>
+    <hyperlink ref="C131" r:id="rId124" xr:uid="{ADB11BDE-27E8-423F-AFDB-5FAAA3892804}"/>
+    <hyperlink ref="C132" r:id="rId125" xr:uid="{DE3934B6-FED0-4609-A6E0-986ABAC1CE69}"/>
+    <hyperlink ref="C134" r:id="rId126" xr:uid="{4156FCA5-20E1-4801-A3EB-FB1100E2354A}"/>
+    <hyperlink ref="C136" r:id="rId127" xr:uid="{1B83D7CB-D69B-498C-9CAC-4BB8F195C9F4}"/>
+    <hyperlink ref="C137" r:id="rId128" xr:uid="{ED7E2358-B5A9-4DA1-89AC-42221E44451D}"/>
+    <hyperlink ref="C138" r:id="rId129" xr:uid="{00B2CF8C-A349-46F9-99D0-73A40EAC8BCD}"/>
+    <hyperlink ref="C139" r:id="rId130" xr:uid="{0168C140-1EBD-4635-A27B-A1F6DB707B99}"/>
+    <hyperlink ref="C140" r:id="rId131" xr:uid="{32E59C3E-FA98-4923-8EE6-5E998F112CE1}"/>
+    <hyperlink ref="C142" r:id="rId132" xr:uid="{50CF528A-B2AD-4844-863A-ED656E183E4D}"/>
+    <hyperlink ref="C133" r:id="rId133" xr:uid="{F6802C6B-31C7-43A4-9758-44BBE446B47A}"/>
+    <hyperlink ref="C135" r:id="rId134" xr:uid="{0E7140E4-72ED-43C7-9ACB-E28E8B6AEBA4}"/>
+    <hyperlink ref="C143" r:id="rId135" xr:uid="{B58922D1-EFBD-4E0F-B032-F3D207B54A16}"/>
+    <hyperlink ref="C145" r:id="rId136" xr:uid="{25F446AC-A40C-4543-890F-2EFC06F6FC1E}"/>
+    <hyperlink ref="C146" r:id="rId137" xr:uid="{3B322F6E-7E7F-4DE7-95E7-C3DBF7ABB633}"/>
+    <hyperlink ref="C147" r:id="rId138" xr:uid="{3ED732A0-1BE2-420B-93EC-8C04838DC24D}"/>
+    <hyperlink ref="C148" r:id="rId139" xr:uid="{6E223FF5-B6CD-4E57-8DBA-4F47D5A4544F}"/>
+    <hyperlink ref="C149" r:id="rId140" xr:uid="{8BA115F0-9A73-4E7E-8C04-39FF7AABC875}"/>
+    <hyperlink ref="C154" r:id="rId141" xr:uid="{C8852A29-E984-41D6-865B-C7F453D536FB}"/>
+    <hyperlink ref="C8" r:id="rId142" xr:uid="{3860EF84-5F21-4F8B-9DA0-1CB4E5991994}"/>
+    <hyperlink ref="C11" r:id="rId143" xr:uid="{DF0B2257-39B5-4A39-8727-C860512B1373}"/>
+    <hyperlink ref="C53" r:id="rId144" xr:uid="{8183C350-9FC9-4B12-BAD5-4152FEE6040A}"/>
+    <hyperlink ref="C63" r:id="rId145" xr:uid="{8AFA7A32-AC5E-4C8E-9937-FF4CF69265DD}"/>
+    <hyperlink ref="C114" r:id="rId146" xr:uid="{A0055B26-2529-4E3C-B7BB-F28D0BA385FF}"/>
+    <hyperlink ref="C70" r:id="rId147" xr:uid="{536A7D39-0A70-4F87-A581-9A9466B014F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
game inner iframe update
</commit_message>
<xml_diff>
--- a/Crawler/App_direct_links.xlsx
+++ b/Crawler/App_direct_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adams\OneDrive\Desktop\Final_Project\Crawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2467DA55-6623-4526-8A09-4AD868AFFA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA740914-7D87-4DB8-B4B6-F6C8B3195CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FINAL" sheetId="16" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2035" uniqueCount="1600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2033" uniqueCount="1600">
   <si>
     <t>Khan Academy</t>
   </si>
@@ -3647,18 +3647,6 @@
     <t xml:space="preserve">https://bellum.io  </t>
   </si>
   <si>
-    <t xml:space="preserve">https://bighunter.io  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://biome3d.com  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.crazygames.com/game/bloxdhop-io  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.crazygames.com/game/bonkio  </t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.crazygames.com/game/buildroyale-io  </t>
   </si>
   <si>
@@ -3866,9 +3854,6 @@
     <t>raised</t>
   </si>
   <si>
-    <t>app-btn-primary</t>
-  </si>
-  <si>
     <t>קישור</t>
   </si>
   <si>
@@ -4787,9 +4772,6 @@
     <t>https://music.youtube.com/watch?v=oWkSspt93XM&amp;list=TLGGpSh6q7XyO6QwNzA3MjAyNQ</t>
   </si>
   <si>
-    <t>btn-play-pulse</t>
-  </si>
-  <si>
     <t>https://www.1001games.com/skill/vex</t>
   </si>
   <si>
@@ -4845,6 +4827,24 @@
   </si>
   <si>
     <t>Gu558e</t>
+  </si>
+  <si>
+    <t>sp_choice_type_11,ready</t>
+  </si>
+  <si>
+    <t>fc-primary-button,btn-play</t>
+  </si>
+  <si>
+    <t>onetrust-accept-btn-handler,btn-play-pulse</t>
+  </si>
+  <si>
+    <t>fc-primary-button,app-btn-primary</t>
+  </si>
+  <si>
+    <t>fc-primary-button,play</t>
+  </si>
+  <si>
+    <t>css-47sehv,play-button</t>
   </si>
 </sst>
 </file>
@@ -9909,13 +9909,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1276</v>
+        <v>1271</v>
       </c>
       <c r="B1" t="s">
-        <v>1275</v>
+        <v>1270</v>
       </c>
       <c r="C1" t="s">
-        <v>1274</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -10435,502 +10435,502 @@
   <sheetData>
     <row r="2" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C2" s="3" t="s">
-        <v>1294</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="3" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
-        <v>1295</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
-        <v>1296</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
-        <v>1297</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
-        <v>1298</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
-        <v>1299</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>1300</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="9" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
-        <v>1301</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="10" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
-        <v>1302</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="11" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
-        <v>1303</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="12" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
-        <v>1304</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="13" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
-        <v>1305</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="14" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
-        <v>1306</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="15" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
-        <v>1307</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="16" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
-        <v>1308</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
-        <v>1309</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
-        <v>1310</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" s="3" t="s">
-        <v>1311</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
-        <v>1312</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21" s="3" t="s">
-        <v>1313</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22" s="3" t="s">
-        <v>1314</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
-        <v>1315</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
-        <v>1316</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C25" s="3" t="s">
-        <v>1317</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="s">
-        <v>1318</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
-        <v>1319</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C28" s="3" t="s">
-        <v>1320</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C29" s="3" t="s">
-        <v>1321</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C30" s="3" t="s">
-        <v>1322</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
-        <v>1323</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C32" s="3" t="s">
-        <v>1324</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="3" t="s">
-        <v>1325</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="3" t="s">
-        <v>1326</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="3" t="s">
-        <v>1327</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" s="3" t="s">
-        <v>1328</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" s="3" t="s">
-        <v>1329</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="s">
-        <v>1330</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" s="3" t="s">
-        <v>1331</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C40" s="3" t="s">
-        <v>1332</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
-        <v>1333</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42" s="3" t="s">
-        <v>1334</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C43" s="3" t="s">
-        <v>1335</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
-        <v>1336</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C45" s="3" t="s">
-        <v>1337</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
-        <v>1338</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C47" s="3" t="s">
-        <v>1339</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C48" s="3" t="s">
-        <v>1340</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" s="3" t="s">
-        <v>1341</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" s="3" t="s">
-        <v>1342</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51" s="3" t="s">
-        <v>1343</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" s="3" t="s">
-        <v>1344</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" s="3" t="s">
-        <v>1345</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" s="3" t="s">
-        <v>1346</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" s="3" t="s">
-        <v>1347</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" s="3" t="s">
-        <v>1348</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" s="3" t="s">
-        <v>1349</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58" s="3" t="s">
-        <v>1350</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" s="3" t="s">
-        <v>1351</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60" s="3" t="s">
-        <v>1352</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" s="3" t="s">
-        <v>1353</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C62" s="3" t="s">
-        <v>1354</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C63" s="3" t="s">
-        <v>1355</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C64" s="3" t="s">
-        <v>1356</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" s="3" t="s">
-        <v>1357</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" s="3" t="s">
-        <v>1358</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C67" s="3" t="s">
-        <v>1359</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" s="3" t="s">
-        <v>1360</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" s="3" t="s">
-        <v>1361</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" s="3" t="s">
-        <v>1362</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C71" s="3" t="s">
-        <v>1363</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" s="3" t="s">
-        <v>1364</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C73" s="3" t="s">
-        <v>1365</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" s="3" t="s">
-        <v>1366</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" s="3" t="s">
-        <v>1367</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" s="3" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" s="3" t="s">
-        <v>1369</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C78" s="3" t="s">
-        <v>1370</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C79" s="3" t="s">
-        <v>1371</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C80" s="3" t="s">
-        <v>1372</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" s="3" t="s">
-        <v>1373</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" s="3" t="s">
-        <v>1374</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" s="3" t="s">
-        <v>1375</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" s="3" t="s">
-        <v>1376</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C85" s="3" t="s">
-        <v>1377</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C86" s="3" t="s">
-        <v>1378</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C87" s="3" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C88" s="3" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C89" s="3" t="s">
-        <v>1381</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C90" s="3" t="s">
-        <v>1382</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C91" s="3" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C92" s="3" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C93" s="3" t="s">
-        <v>1385</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C94" s="3" t="s">
-        <v>1386</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C95" s="3" t="s">
-        <v>1387</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C96" s="3" t="s">
-        <v>1388</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" s="3" t="s">
-        <v>1389</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" s="3" t="s">
-        <v>1390</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="3" t="s">
-        <v>1391</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" s="3" t="s">
-        <v>1392</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" s="3" t="s">
-        <v>1393</v>
+        <v>1388</v>
       </c>
     </row>
   </sheetData>
@@ -10954,7 +10954,7 @@
   <sheetData>
     <row r="2" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C2" s="5" t="s">
-        <v>1394</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="3" spans="3:3" x14ac:dyDescent="0.3">
@@ -10964,42 +10964,42 @@
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
-        <v>1395</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C5" s="5" t="s">
-        <v>1396</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
-        <v>1397</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C7" s="5" t="s">
-        <v>1398</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C8" s="5" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="9" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="10" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C10" s="5" t="s">
-        <v>1401</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="11" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
-        <v>1402</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="12" spans="3:3" x14ac:dyDescent="0.3">
@@ -11014,7 +11014,7 @@
     </row>
     <row r="14" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C14" s="5" t="s">
-        <v>1403</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="15" spans="3:3" x14ac:dyDescent="0.3">
@@ -11024,12 +11024,12 @@
     </row>
     <row r="16" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C16" s="5" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="5" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
@@ -11039,417 +11039,417 @@
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" s="5" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" s="5" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21" s="5" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22" s="5" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C23" s="5" t="s">
-        <v>1410</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C24" s="5" t="s">
-        <v>1411</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C25" s="5" t="s">
-        <v>1412</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C26" s="5" t="s">
-        <v>1413</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C27" s="5" t="s">
-        <v>1414</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C28" s="5" t="s">
-        <v>1415</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C29" s="5" t="s">
-        <v>1416</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C30" s="5" t="s">
-        <v>1417</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C31" s="5" t="s">
-        <v>1418</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C32" s="5" t="s">
-        <v>1419</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="5" t="s">
-        <v>1420</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="5" t="s">
-        <v>1421</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="5" t="s">
-        <v>1422</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" s="5" t="s">
-        <v>1423</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" s="5" t="s">
-        <v>1424</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" s="5" t="s">
-        <v>1425</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" s="5" t="s">
-        <v>1426</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C40" s="5" t="s">
-        <v>1427</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C41" s="5" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42" s="5" t="s">
-        <v>1429</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C43" s="5" t="s">
-        <v>1430</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C44" s="5" t="s">
-        <v>1431</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C45" s="5" t="s">
-        <v>1432</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C46" s="5" t="s">
-        <v>1433</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C47" s="5" t="s">
-        <v>1434</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C48" s="5" t="s">
-        <v>1435</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" s="5" t="s">
-        <v>1436</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" s="5" t="s">
-        <v>1437</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51" s="5" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" s="5" t="s">
-        <v>1439</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" s="5" t="s">
-        <v>1440</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" s="5" t="s">
-        <v>1441</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" s="5" t="s">
-        <v>1442</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" s="5" t="s">
-        <v>1443</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" s="5" t="s">
-        <v>1444</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58" s="5" t="s">
-        <v>1445</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" s="5" t="s">
-        <v>1446</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60" s="5" t="s">
-        <v>1447</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" s="5" t="s">
-        <v>1448</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C62" s="5" t="s">
-        <v>1449</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C63" s="5" t="s">
-        <v>1450</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C64" s="5" t="s">
-        <v>1451</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" s="5" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" s="5" t="s">
-        <v>1453</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C67" s="5" t="s">
-        <v>1454</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" s="5" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" s="5" t="s">
-        <v>1456</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" s="5" t="s">
-        <v>1457</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C71" s="5" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" s="5" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C73" s="5" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" s="5" t="s">
-        <v>1461</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" s="5" t="s">
-        <v>1462</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" s="5" t="s">
-        <v>1463</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" s="5" t="s">
-        <v>1464</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C78" s="5" t="s">
-        <v>1465</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C79" s="5" t="s">
-        <v>1466</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C80" s="5" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" s="5" t="s">
-        <v>1468</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" s="5" t="s">
-        <v>1469</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" s="5" t="s">
-        <v>1470</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" s="5" t="s">
-        <v>1471</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C85" s="5" t="s">
-        <v>1472</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C86" s="5" t="s">
-        <v>1473</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C87" s="5" t="s">
-        <v>1474</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C88" s="5" t="s">
-        <v>1475</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C89" s="5" t="s">
-        <v>1476</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C90" s="5" t="s">
-        <v>1477</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C91" s="5" t="s">
-        <v>1478</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C92" s="5" t="s">
-        <v>1479</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C93" s="5" t="s">
-        <v>1480</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C94" s="5" t="s">
-        <v>1481</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C95" s="5" t="s">
-        <v>1431</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C96" s="5" t="s">
-        <v>1415</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" s="5" t="s">
-        <v>1482</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" s="5" t="s">
-        <v>1483</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="5" t="s">
-        <v>1484</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" s="5" t="s">
-        <v>1485</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" s="5" t="s">
-        <v>1432</v>
+        <v>1427</v>
       </c>
     </row>
   </sheetData>
@@ -11474,13 +11474,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1276</v>
+        <v>1271</v>
       </c>
       <c r="B1" t="s">
-        <v>1275</v>
+        <v>1270</v>
       </c>
       <c r="C1" t="s">
-        <v>1274</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -11522,7 +11522,7 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="3" t="s">
-        <v>1489</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -11554,7 +11554,7 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="3" t="s">
-        <v>1596</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -11575,7 +11575,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" s="14" t="s">
-        <v>1501</v>
+        <v>1496</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>864</v>
@@ -11592,7 +11592,7 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" s="18"/>
       <c r="C19" s="3" t="s">
-        <v>1502</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -11603,7 +11603,7 @@
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="21"/>
       <c r="B21" s="14" t="s">
-        <v>1278</v>
+        <v>1273</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>971</v>
@@ -11611,7 +11611,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" s="14" t="s">
-        <v>1277</v>
+        <v>1272</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>884</v>
@@ -11633,7 +11633,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
-        <v>1286</v>
+        <v>1281</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>886</v>
@@ -11641,7 +11641,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" s="18" t="s">
-        <v>1279</v>
+        <v>1274</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>873</v>
@@ -11654,10 +11654,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" s="18" t="s">
-        <v>1501</v>
+        <v>1496</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>1487</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -11675,7 +11675,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" s="18" t="s">
-        <v>1280</v>
+        <v>1275</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>881</v>
@@ -11705,7 +11705,7 @@
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
       <c r="B36" s="18" t="s">
-        <v>1282</v>
+        <v>1277</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>897</v>
@@ -11713,7 +11713,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" s="18" t="s">
-        <v>1283</v>
+        <v>1278</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>898</v>
@@ -11721,7 +11721,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B38" s="18" t="s">
-        <v>1284</v>
+        <v>1279</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>899</v>
@@ -11734,7 +11734,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" s="18" t="s">
-        <v>1285</v>
+        <v>1280</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>901</v>
@@ -11752,7 +11752,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="18" t="s">
-        <v>1287</v>
+        <v>1282</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>906</v>
@@ -11776,7 +11776,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" s="18" t="s">
-        <v>1288</v>
+        <v>1283</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>912</v>
@@ -11789,7 +11789,7 @@
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="18" t="s">
-        <v>1289</v>
+        <v>1284</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>916</v>
@@ -11802,7 +11802,7 @@
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="18" t="s">
-        <v>1290</v>
+        <v>1285</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>919</v>
@@ -11816,7 +11816,7 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" s="18" t="s">
-        <v>1291</v>
+        <v>1286</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>924</v>
@@ -11829,10 +11829,10 @@
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" s="18" t="s">
-        <v>1293</v>
+        <v>1288</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>1292</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.3">
@@ -11882,36 +11882,36 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B65" s="18" t="s">
-        <v>1503</v>
+        <v>1498</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>1486</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>1521</v>
+        <v>1516</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>1519</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C67" s="5" t="s">
-        <v>1571</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C68" s="5" t="s">
-        <v>1578</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>1573</v>
+        <v>1568</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>1572</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.3">
@@ -12051,7 +12051,7 @@
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C97" s="22" t="s">
-        <v>1281</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.3">
@@ -12166,7 +12166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FC6163-F89F-44E5-90BE-4CFB44CF1FB4}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
@@ -12179,18 +12179,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1518</v>
+        <v>1513</v>
       </c>
       <c r="B1" t="s">
-        <v>1275</v>
+        <v>1270</v>
       </c>
       <c r="C1" t="s">
-        <v>1274</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
-        <v>1488</v>
+        <v>1483</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>940</v>
@@ -12198,7 +12198,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
-        <v>1490</v>
+        <v>1485</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>941</v>
@@ -12206,7 +12206,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
-        <v>1491</v>
+        <v>1486</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>943</v>
@@ -12214,7 +12214,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>1585</v>
+        <v>1579</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>944</v>
@@ -12222,18 +12222,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1515</v>
+        <v>1510</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>1546</v>
+        <v>1541</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1586</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>1587</v>
+        <v>1581</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>946</v>
@@ -12241,15 +12241,15 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
-        <v>1492</v>
+        <v>1487</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1588</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
-        <v>1493</v>
+        <v>1488</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>948</v>
@@ -12257,10 +12257,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1589</v>
+        <v>1583</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>1494</v>
+        <v>1489</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>949</v>
@@ -12268,7 +12268,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
-        <v>1560</v>
+        <v>1555</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>950</v>
@@ -12276,15 +12276,15 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
-        <v>1591</v>
+        <v>1585</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1590</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
-        <v>1495</v>
+        <v>1490</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>953</v>
@@ -12292,7 +12292,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>1496</v>
+        <v>1491</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>954</v>
@@ -12300,7 +12300,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
-        <v>1497</v>
+        <v>1492</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>955</v>
@@ -12308,7 +12308,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
-        <v>1498</v>
+        <v>1493</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>963</v>
@@ -12316,7 +12316,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" s="18" t="s">
-        <v>1499</v>
+        <v>1494</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>956</v>
@@ -12324,7 +12324,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>1500</v>
+        <v>1495</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>957</v>
@@ -12332,7 +12332,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
-        <v>1504</v>
+        <v>1499</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>923</v>
@@ -12340,7 +12340,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" s="18" t="s">
-        <v>1505</v>
+        <v>1500</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>958</v>
@@ -12348,7 +12348,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
-        <v>1506</v>
+        <v>1501</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>959</v>
@@ -12356,7 +12356,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
-        <v>1507</v>
+        <v>1502</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>960</v>
@@ -12364,15 +12364,15 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" s="18" t="s">
-        <v>1509</v>
+        <v>1504</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>1508</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" s="18" t="s">
-        <v>1510</v>
+        <v>1505</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>931</v>
@@ -12380,7 +12380,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
-        <v>1511</v>
+        <v>1506</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>933</v>
@@ -12388,7 +12388,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" s="18" t="s">
-        <v>1512</v>
+        <v>1507</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>915</v>
@@ -12401,7 +12401,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" s="18" t="s">
-        <v>1513</v>
+        <v>1508</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>929</v>
@@ -12409,7 +12409,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1514</v>
+        <v>1509</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="5" t="s">
@@ -12418,7 +12418,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" s="18" t="s">
-        <v>1516</v>
+        <v>1511</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>887</v>
@@ -12426,7 +12426,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" s="18" t="s">
-        <v>1517</v>
+        <v>1512</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>893</v>
@@ -12434,18 +12434,18 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
-        <v>1527</v>
+        <v>1522</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>1520</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1522</v>
+        <v>1517</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>1505</v>
+        <v>1500</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>908</v>
@@ -12453,7 +12453,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" s="18" t="s">
-        <v>1523</v>
+        <v>1518</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>910</v>
@@ -12461,7 +12461,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" s="18" t="s">
-        <v>1524</v>
+        <v>1519</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>913</v>
@@ -12469,7 +12469,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="18" t="s">
-        <v>1558</v>
+        <v>1553</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>865</v>
@@ -12477,7 +12477,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" s="18" t="s">
-        <v>1525</v>
+        <v>1520</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>970</v>
@@ -12485,15 +12485,15 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B38" s="18" t="s">
-        <v>1593</v>
+        <v>1587</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>1592</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B39" s="18" t="s">
-        <v>1526</v>
+        <v>1521</v>
       </c>
       <c r="C39" s="26" t="s">
         <v>972</v>
@@ -12501,29 +12501,29 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" s="18" t="s">
-        <v>1529</v>
+        <v>1524</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1528</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41" s="18" t="s">
-        <v>1531</v>
+        <v>1526</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>1530</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="25"/>
       <c r="C42" s="9" t="s">
-        <v>1532</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="18" t="s">
-        <v>1533</v>
+        <v>1528</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>706</v>
@@ -12531,7 +12531,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="18" t="s">
-        <v>1534</v>
+        <v>1529</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>710</v>
@@ -12539,7 +12539,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="18" t="s">
-        <v>1535</v>
+        <v>1530</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>711</v>
@@ -12547,7 +12547,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="18" t="s">
-        <v>1536</v>
+        <v>1531</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>712</v>
@@ -12555,45 +12555,45 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" s="18" t="s">
-        <v>1538</v>
+        <v>1533</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>1537</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B48" s="18"/>
       <c r="C48" s="9" t="s">
-        <v>1539</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="18" t="s">
-        <v>1541</v>
+        <v>1536</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>1540</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="18" t="s">
-        <v>1543</v>
+        <v>1538</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>1542</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="18" t="s">
-        <v>1534</v>
+        <v>1529</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>1594</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="18" t="s">
-        <v>1544</v>
+        <v>1539</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>717</v>
@@ -12601,55 +12601,55 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" s="18" t="s">
-        <v>1546</v>
+        <v>1541</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>1545</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" s="18" t="s">
-        <v>1548</v>
+        <v>1543</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>1547</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" s="18" t="s">
-        <v>1550</v>
+        <v>1545</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>1549</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" s="18" t="s">
-        <v>1557</v>
+        <v>1552</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>1551</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" s="18" t="s">
-        <v>1517</v>
+        <v>1512</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>1552</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" s="18" t="s">
-        <v>1595</v>
+        <v>1589</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>1553</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" s="18" t="s">
-        <v>1554</v>
+        <v>1549</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>737</v>
@@ -12658,20 +12658,20 @@
     <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B60" s="18"/>
       <c r="C60" s="9" t="s">
-        <v>1555</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B61" s="18" t="s">
-        <v>1559</v>
+        <v>1554</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>1556</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B62" s="18" t="s">
-        <v>1561</v>
+        <v>1556</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>740</v>
@@ -12679,7 +12679,7 @@
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B63" s="18" t="s">
-        <v>1562</v>
+        <v>1557</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>741</v>
@@ -12687,12 +12687,12 @@
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C64" s="9" t="s">
-        <v>1563</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B65" s="18" t="s">
-        <v>1564</v>
+        <v>1559</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>743</v>
@@ -12700,50 +12700,50 @@
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B66" s="18" t="s">
-        <v>1566</v>
+        <v>1561</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>1565</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B67" s="18" t="s">
-        <v>1568</v>
+        <v>1563</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>1567</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B68" s="18" t="s">
-        <v>1570</v>
+        <v>1565</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>1569</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B69" s="18" t="s">
-        <v>1575</v>
+        <v>1570</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>1574</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>1577</v>
+        <v>1572</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>1576</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B71" s="18" t="s">
-        <v>1599</v>
+        <v>1593</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>1579</v>
+        <v>1574</v>
       </c>
     </row>
   </sheetData>
@@ -12786,13 +12786,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1276</v>
+        <v>1271</v>
       </c>
       <c r="B1" t="s">
-        <v>1275</v>
+        <v>1270</v>
       </c>
       <c r="C1" t="s">
-        <v>1274</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -13312,13 +13312,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1276</v>
+        <v>1271</v>
       </c>
       <c r="B1" t="s">
-        <v>1275</v>
+        <v>1270</v>
       </c>
       <c r="C1" t="s">
-        <v>1274</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -13852,13 +13852,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1276</v>
+        <v>1271</v>
       </c>
       <c r="B1" t="s">
-        <v>1275</v>
+        <v>1270</v>
       </c>
       <c r="C1" t="s">
-        <v>1274</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -14674,10 +14674,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F2D1A5-2BF6-4BAC-B823-F864749CEE0B}">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14687,18 +14687,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1276</v>
+        <v>1271</v>
       </c>
       <c r="B1" t="s">
-        <v>1275</v>
+        <v>1270</v>
       </c>
       <c r="C1" t="s">
-        <v>1274</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1188</v>
@@ -14706,7 +14706,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>967</v>
+        <v>1595</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1189</v>
@@ -14714,15 +14714,15 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
-        <v>1580</v>
+        <v>1596</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1581</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>1273</v>
+        <v>1597</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1193</v>
@@ -14730,7 +14730,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>1517</v>
+        <v>1598</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1194</v>
@@ -14743,7 +14743,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>1582</v>
+        <v>1576</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1196</v>
@@ -14751,7 +14751,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>1517</v>
+        <v>1512</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1197</v>
@@ -14759,7 +14759,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>1597</v>
+        <v>1591</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>1198</v>
@@ -14767,26 +14767,32 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>1584</v>
+        <v>1578</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>1583</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>1598</v>
+        <v>1592</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1199</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>1594</v>
+      </c>
       <c r="C13" s="3" t="s">
         <v>1200</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>1599</v>
+      </c>
       <c r="C14" s="3" t="s">
         <v>1201</v>
       </c>
@@ -15123,41 +15129,21 @@
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" s="3" t="s">
-        <v>1268</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" s="3" t="s">
-        <v>1269</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" s="3" t="s">
-        <v>1270</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" s="3" t="s">
-        <v>1271</v>
-      </c>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C85" s="3" t="s">
-        <v>1187</v>
-      </c>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C86" s="3" t="s">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C87" s="3" t="s">
-        <v>1191</v>
-      </c>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C88" s="3" t="s">
         <v>1192</v>
       </c>
     </row>
@@ -15167,8 +15153,9 @@
     <hyperlink ref="C7" r:id="rId2" xr:uid="{40005C80-7A70-4BCF-A7F3-9C311088CA3A}"/>
     <hyperlink ref="C8" r:id="rId3" xr:uid="{85D8E411-ABE9-4167-AD9F-53691417C7A8}"/>
     <hyperlink ref="C9" r:id="rId4" xr:uid="{CF68C9D5-876B-4B78-83D8-52D944A2E1D7}"/>
+    <hyperlink ref="C13" r:id="rId5" xr:uid="{BB57683D-7C51-49E3-B55A-EE593E4D5998}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
game inner iframe shadow root
</commit_message>
<xml_diff>
--- a/Crawler/App_direct_links.xlsx
+++ b/Crawler/App_direct_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adams\OneDrive\Desktop\Final_Project\Crawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA740914-7D87-4DB8-B4B6-F6C8B3195CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD94845-D167-46D1-B61D-F1E0860748C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FINAL" sheetId="16" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2033" uniqueCount="1600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2039" uniqueCount="1605">
   <si>
     <t>Khan Academy</t>
   </si>
@@ -4844,7 +4844,22 @@
     <t>fc-primary-button,play</t>
   </si>
   <si>
-    <t>css-47sehv,play-button</t>
+    <t>css-47sehv</t>
+  </si>
+  <si>
+    <t>onetrust-accept-btn-handler,admeen-splash-button,gd__skip__ad</t>
+  </si>
+  <si>
+    <t>fc-primary-button,playbtn</t>
+  </si>
+  <si>
+    <t>fc-primary-button,</t>
+  </si>
+  <si>
+    <t>fc-primary-button,spawn-button</t>
+  </si>
+  <si>
+    <t>.cb-i</t>
   </si>
 </sst>
 </file>
@@ -14674,10 +14689,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F2D1A5-2BF6-4BAC-B823-F864749CEE0B}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14685,7 +14700,7 @@
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1271</v>
       </c>
@@ -14696,7 +14711,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1268</v>
       </c>
@@ -14704,7 +14719,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1595</v>
       </c>
@@ -14712,450 +14727,473 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
-        <v>1596</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>1597</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1575</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>1193</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>1598</v>
-      </c>
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
-        <v>1194</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>1576</v>
+      </c>
       <c r="C7" s="3" t="s">
-        <v>1195</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>1576</v>
+        <v>1512</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>1196</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>1512</v>
+        <v>1591</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>1591</v>
+        <v>1578</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1577</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>1578</v>
+        <v>1592</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>1577</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>1592</v>
+        <v>1601</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1604</v>
+      </c>
       <c r="B13" t="s">
-        <v>1594</v>
+        <v>1603</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>1599</v>
-      </c>
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
-        <v>1201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
-        <v>1203</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
-        <v>1204</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
-        <v>1205</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" s="3" t="s">
-        <v>1206</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
-        <v>1207</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21" s="3" t="s">
-        <v>1208</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22" s="3" t="s">
-        <v>1209</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
-        <v>1210</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
-        <v>1211</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C25" s="3" t="s">
-        <v>1212</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="s">
-        <v>1213</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
-        <v>1214</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C28" s="3" t="s">
-        <v>1215</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C29" s="3" t="s">
-        <v>1216</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C30" s="3" t="s">
-        <v>1217</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
-        <v>1218</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C32" s="3" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="3" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C35" s="3" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="3" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C38" s="3" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="3" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C40" s="3" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C41" s="3" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C42" s="3" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C43" s="3" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="3" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="3" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C46" s="3" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C47" s="3" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C48" s="3" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="3" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="3" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C52" s="3" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>1600</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C54" s="3" t="s">
         <v>1219</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="3" t="s">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="3" t="s">
-        <v>1221</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="3" t="s">
-        <v>1222</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="3" t="s">
-        <v>1223</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="3" t="s">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="3" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="3" t="s">
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" s="3" t="s">
-        <v>1227</v>
-      </c>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C41" s="3" t="s">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C42" s="3" t="s">
-        <v>1229</v>
-      </c>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C43" s="3" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C44" s="3" t="s">
-        <v>1231</v>
-      </c>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C45" s="3" t="s">
-        <v>1232</v>
-      </c>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C46" s="3" t="s">
-        <v>1233</v>
-      </c>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C47" s="3" t="s">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C55" s="3" t="s">
         <v>1234</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C48" s="3" t="s">
-        <v>1235</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="3" t="s">
-        <v>1236</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C50" s="3" t="s">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C51" s="3" t="s">
-        <v>1238</v>
-      </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C52" s="3" t="s">
-        <v>1239</v>
-      </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C53" s="3" t="s">
-        <v>1240</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C54" s="3" t="s">
-        <v>1241</v>
-      </c>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C55" s="3" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C56" s="3" t="s">
-        <v>1243</v>
-      </c>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C57" s="3" t="s">
-        <v>1244</v>
-      </c>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C58" s="3" t="s">
-        <v>1245</v>
-      </c>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="20" t="s">
+        <v>1596</v>
+      </c>
       <c r="C59" s="3" t="s">
-        <v>1246</v>
-      </c>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C60" s="3" t="s">
-        <v>1247</v>
-      </c>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C61" s="3" t="s">
-        <v>1248</v>
-      </c>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>1594</v>
+      </c>
       <c r="C62" s="3" t="s">
-        <v>1249</v>
-      </c>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C63" s="3" t="s">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C64" s="3" t="s">
-        <v>1251</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" s="3" t="s">
-        <v>1252</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" s="3" t="s">
-        <v>1253</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C67" s="3" t="s">
-        <v>1254</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" s="3" t="s">
-        <v>1255</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" s="3" t="s">
-        <v>1256</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" s="3" t="s">
-        <v>1257</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C71" s="3" t="s">
-        <v>1258</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" s="3" t="s">
-        <v>1259</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C73" s="3" t="s">
-        <v>1260</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" s="3" t="s">
-        <v>1261</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" s="3" t="s">
-        <v>1262</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" s="3" t="s">
-        <v>1263</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" s="3" t="s">
-        <v>1264</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C78" s="3" t="s">
-        <v>1265</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C79" s="3" t="s">
-        <v>1266</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C80" s="3" t="s">
-        <v>1267</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" s="3" t="s">
-        <v>1187</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" s="3" t="s">
-        <v>1190</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" s="3" t="s">
-        <v>1191</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" s="3" t="s">
-        <v>1192</v>
+        <v>1267</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C84">
+    <sortCondition ref="C1:C84"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{6FEEC0A2-C760-4642-9FCE-AA70BD4747B2}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{40005C80-7A70-4BCF-A7F3-9C311088CA3A}"/>
-    <hyperlink ref="C8" r:id="rId3" xr:uid="{85D8E411-ABE9-4167-AD9F-53691417C7A8}"/>
-    <hyperlink ref="C9" r:id="rId4" xr:uid="{CF68C9D5-876B-4B78-83D8-52D944A2E1D7}"/>
-    <hyperlink ref="C13" r:id="rId5" xr:uid="{BB57683D-7C51-49E3-B55A-EE593E4D5998}"/>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{6FEEC0A2-C760-4642-9FCE-AA70BD4747B2}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{40005C80-7A70-4BCF-A7F3-9C311088CA3A}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{85D8E411-ABE9-4167-AD9F-53691417C7A8}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{CF68C9D5-876B-4B78-83D8-52D944A2E1D7}"/>
+    <hyperlink ref="C62" r:id="rId5" xr:uid="{BB57683D-7C51-49E3-B55A-EE593E4D5998}"/>
+    <hyperlink ref="C12" r:id="rId6" xr:uid="{2DC01A65-051F-48E2-8B3E-D1D5B13A0504}"/>
+    <hyperlink ref="C13" r:id="rId7" xr:uid="{53139477-658F-4079-A39F-4225264C18E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
125 in games & browsers
</commit_message>
<xml_diff>
--- a/Crawler/App_direct_links.xlsx
+++ b/Crawler/App_direct_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Desktop\Final_Project\Crawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B407DC57-10E1-4ECF-94E6-4CBCD985407B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331725EA-390D-4BAB-BA7E-A762F624C8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Video Str." sheetId="17" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="1057">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="1115">
   <si>
     <t>https://www.1001freefonts.com/</t>
   </si>
@@ -3210,6 +3210,180 @@
   </si>
   <si>
     <t>https://earth.google.com/web/@32.1050935,34.8934402,26.79523346a,31570.60219207d,35y,0h,0t,0r/data=CgRCAggBOgMKATBCAggASg0I____________ARAA?authuser=0</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/spot-the-differences</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/diva-hair-salon</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/cozy-room-design</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/wacky-doodle-fixes</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/stupidella-horror</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/dual-cat-max</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/sushi-merge</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/who-is</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/star-blogger-left-or-right</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/beauty-salon</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/sweet-ball-sprint</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/hide-and-seek-escape-games</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/prankster-3d</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/subway-surfers</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/horror-dungeon-3d</t>
+  </si>
+  <si>
+    <t>https://poki.com/fr/g/la-petite-avril</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/arcane-archer</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/snow-plow</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/digging-master</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/smash-it</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/fishing-league</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/cube-miner-escape-from-prison</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/gold-digger-frvr</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/village-craft</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/iron-snout</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/survival-island</t>
+  </si>
+  <si>
+    <t>https://poki.com/en/g/fantasy-sandbox</t>
+  </si>
+  <si>
+    <t>https://radioparadise.com/</t>
+  </si>
+  <si>
+    <t>https://jazzradio.com/</t>
+  </si>
+  <si>
+    <t>https://www.classicalradio.com/</t>
+  </si>
+  <si>
+    <t>https://live365.com/</t>
+  </si>
+  <si>
+    <t>https://www.fipradio.fr/</t>
+  </si>
+  <si>
+    <t>https://abcnewsradio.co/</t>
+  </si>
+  <si>
+    <t>https://dashradio.com/</t>
+  </si>
+  <si>
+    <t>https://www.kcrw.com/</t>
+  </si>
+  <si>
+    <t>https://www.kexp.org/</t>
+  </si>
+  <si>
+    <t>https://wfmu.org/</t>
+  </si>
+  <si>
+    <t>https://ancientfm.com/</t>
+  </si>
+  <si>
+    <t>https://www.aljazeera.com/live/</t>
+  </si>
+  <si>
+    <t>https://www.rfi.fr/en/english/</t>
+  </si>
+  <si>
+    <t>https://www.voanews.com/audio</t>
+  </si>
+  <si>
+    <t>https://www.jamendo.com/start</t>
+  </si>
+  <si>
+    <t>https://hearthis.at/</t>
+  </si>
+  <si>
+    <t>https://ocremix.org/</t>
+  </si>
+  <si>
+    <t>https://relisten.net/</t>
+  </si>
+  <si>
+    <t>https://archive.org/details/live_music_archive</t>
+  </si>
+  <si>
+    <t>https://zeno.fm/</t>
+  </si>
+  <si>
+    <t>https://noisli.com/</t>
+  </si>
+  <si>
+    <t>https://coffitivity.com/</t>
+  </si>
+  <si>
+    <t>https://ambientsleepingpill.com/</t>
+  </si>
+  <si>
+    <t>https://www.liveatc.net/</t>
+  </si>
+  <si>
+    <t>https://www.broadcastify.com/</t>
+  </si>
+  <si>
+    <t>http://websdr.org/</t>
+  </si>
+  <si>
+    <t>https://podbay.fm/</t>
+  </si>
+  <si>
+    <t>https://librivox.org/</t>
+  </si>
+  <si>
+    <t>https://www.storynory.com/</t>
+  </si>
+  <si>
+    <t>https://forvo.com/</t>
+  </si>
+  <si>
+    <t>https://rainwave.cc/</t>
   </si>
 </sst>
 </file>
@@ -5554,10 +5728,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31A2EFD-A127-47E5-B375-5235669A0921}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5575,212 +5749,212 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>104</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>105</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>106</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>107</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>108</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>109</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>110</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>111</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>112</v>
+        <v>987</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>113</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>114</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>115</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>116</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>117</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>118</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>119</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>120</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>121</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>122</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>123</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>124</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>125</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>126</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>130</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>131</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>133</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>135</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>137</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>139</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>143</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>144</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>145</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.25">
@@ -5790,290 +5964,463 @@
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>147</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>150</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>154</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>157</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>161</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>168</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>174</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>177</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>178</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>179</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>181</v>
+        <v>125</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>184</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>185</v>
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
-        <v>187</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
-        <v>193</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>194</v>
+        <v>127</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
-        <v>195</v>
+        <v>133</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
-        <v>196</v>
+        <v>119</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
-        <v>198</v>
+        <v>142</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
-        <v>200</v>
+        <v>117</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
-        <v>201</v>
+        <v>168</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" t="s">
-        <v>203</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C127" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C131" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C133" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C135" t="s">
+        <v>1103</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C135">
+    <sortCondition ref="C62:C135"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7410,10 +7757,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F2D1A5-2BF6-4BAC-B823-F864749CEE0B}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C128"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7547,7 +7894,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>357</v>
       </c>
@@ -7555,110 +7902,98 @@
         <v>453</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>90</v>
-      </c>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>396</v>
+        <v>439</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>439</v>
-      </c>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>367</v>
+      </c>
       <c r="C21" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>30</v>
-      </c>
+        <v>471</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>481</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>367</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>461</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>481</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="9" t="s">
-        <v>468</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>434</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>367</v>
-      </c>
-      <c r="C28" s="2" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="4" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C30" s="2" t="s">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C32" s="2" t="s">
         <v>502</v>
       </c>
@@ -7699,351 +8034,501 @@
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="3" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="3" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C41" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C42" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C43" s="2" t="s">
-        <v>497</v>
-      </c>
-    </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C44" s="4" t="s">
-        <v>508</v>
+      <c r="C44" s="3" t="s">
+        <v>1058</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="4" t="s">
-        <v>507</v>
+        <v>526</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C46" s="4" t="s">
-        <v>532</v>
+      <c r="C46" s="3" t="s">
+        <v>1062</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C47" s="4" t="s">
-        <v>531</v>
+      <c r="C47" s="2" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" s="2" t="s">
-        <v>489</v>
+      <c r="C49" s="3" t="s">
+        <v>1083</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" s="2" t="s">
-        <v>485</v>
+      <c r="C50" s="3" t="s">
+        <v>1077</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="4" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="4" t="s">
-        <v>525</v>
+        <v>507</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="4" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" s="2" t="s">
-        <v>506</v>
+      <c r="C54" s="3" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="4" t="s">
-        <v>515</v>
+        <v>531</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="2" t="s">
-        <v>319</v>
+        <v>485</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C59" s="2" t="s">
-        <v>496</v>
+      <c r="C59" s="3" t="s">
+        <v>1068</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C60" s="2" t="s">
-        <v>442</v>
+      <c r="C60" s="3" t="s">
+        <v>1071</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="4" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="4" t="s">
-        <v>520</v>
+        <v>525</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C63" s="2" t="s">
-        <v>490</v>
+      <c r="C63" s="4" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C64" s="4" t="s">
-        <v>523</v>
+      <c r="C64" s="2" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65" s="2" t="s">
-        <v>488</v>
+      <c r="C65" s="3" t="s">
+        <v>1081</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C66" s="2" t="s">
-        <v>500</v>
+      <c r="C66" s="4" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C68" s="4" t="s">
-        <v>516</v>
+      <c r="C68" s="2" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C69" s="4" t="s">
-        <v>514</v>
+      <c r="C69" s="2" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C71" s="4" t="s">
-        <v>510</v>
+      <c r="C71" s="2" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C72" s="2" t="s">
-        <v>486</v>
+      <c r="C72" s="4" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" s="4" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C75" s="2" t="s">
-        <v>493</v>
+      <c r="C75" s="4" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" s="2" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="4" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="4" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="4" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="3" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="4" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="3" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="3" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="4" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C78" s="4" t="s">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C93" s="3" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="4" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C79" s="2" t="s">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C80" s="2" t="s">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="2" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C81" s="4" t="s">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="4" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C82" s="4" t="s">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="3" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="3" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="4" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C83" s="4" t="s">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="3" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="3" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="4" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="4" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C84" s="2" t="s">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="2" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C85" s="2" t="s">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="3" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="2" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C86" s="4" t="s">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="3" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C109" s="4" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C87" s="2" t="s">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="2" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C111" s="3" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C112" s="3" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
         <v>367</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
         <v>445</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C90" s="2" t="s">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C115" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C91" s="2" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C116" s="2" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
         <v>424</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>1</v>
+      </c>
+      <c r="B118" t="s">
         <v>473</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
         <v>452</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C95" s="2" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C120" s="2" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
         <v>437</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C97" s="2" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C122" s="2" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
         <v>447</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C123" s="2" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
         <v>447</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C124" s="2" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
         <v>457</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C125" s="2" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
         <v>50</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B126" t="s">
         <v>479</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C126" s="2" t="s">
         <v>478</v>
       </c>
     </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>90</v>
+      </c>
+      <c r="B127" t="s">
+        <v>396</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>30</v>
+      </c>
+      <c r="B128" t="s">
+        <v>466</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C101">
-    <sortCondition ref="C70:C101"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C126">
+    <sortCondition ref="C69:C126"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" xr:uid="{6FEEC0A2-C760-4642-9FCE-AA70BD4747B2}"/>
@@ -8052,83 +8537,85 @@
     <hyperlink ref="C9" r:id="rId4" xr:uid="{CF68C9D5-876B-4B78-83D8-52D944A2E1D7}"/>
     <hyperlink ref="C16" r:id="rId5" xr:uid="{2DC01A65-051F-48E2-8B3E-D1D5B13A0504}"/>
     <hyperlink ref="C11" r:id="rId6" xr:uid="{AC17905D-C1F3-4794-8E92-F209F68B3FA3}"/>
-    <hyperlink ref="C42" r:id="rId7" xr:uid="{77F9D3AF-224B-47FC-8BBE-DE7CA37B8727}"/>
+    <hyperlink ref="C47" r:id="rId7" xr:uid="{77F9D3AF-224B-47FC-8BBE-DE7CA37B8727}"/>
     <hyperlink ref="C15" r:id="rId8" xr:uid="{797BEB4C-AF16-4C98-A229-5103EDBA229D}"/>
-    <hyperlink ref="C99" r:id="rId9" xr:uid="{DE4D6B01-BE21-4C68-9BBB-A1E2022D24DA}"/>
-    <hyperlink ref="C27" r:id="rId10" xr:uid="{BEAF85A1-638D-4FD9-A592-2ED097CE9B8A}"/>
-    <hyperlink ref="C20" r:id="rId11" xr:uid="{EB5D17FA-B684-4C02-8A35-989CA6469612}"/>
-    <hyperlink ref="C98" r:id="rId12" xr:uid="{C278573D-D2FD-492E-813A-9DA9B30825F8}"/>
-    <hyperlink ref="C21" r:id="rId13" location="/game/{%22currentRoomId%22:%22349b25cd-d363-595d-cdf8-1df483fa2927%22}" xr:uid="{82704D4A-2ABB-4A1F-9B31-3AB510DA1CE4}"/>
-    <hyperlink ref="C24" r:id="rId14" xr:uid="{D3775193-2D86-4350-82E0-3967E80848EF}"/>
+    <hyperlink ref="C124" r:id="rId9" xr:uid="{DE4D6B01-BE21-4C68-9BBB-A1E2022D24DA}"/>
+    <hyperlink ref="C25" r:id="rId10" xr:uid="{BEAF85A1-638D-4FD9-A592-2ED097CE9B8A}"/>
+    <hyperlink ref="C19" r:id="rId11" xr:uid="{EB5D17FA-B684-4C02-8A35-989CA6469612}"/>
+    <hyperlink ref="C123" r:id="rId12" xr:uid="{C278573D-D2FD-492E-813A-9DA9B30825F8}"/>
+    <hyperlink ref="C20" r:id="rId13" location="/game/{%22currentRoomId%22:%22349b25cd-d363-595d-cdf8-1df483fa2927%22}" xr:uid="{82704D4A-2ABB-4A1F-9B31-3AB510DA1CE4}"/>
+    <hyperlink ref="C22" r:id="rId14" xr:uid="{D3775193-2D86-4350-82E0-3967E80848EF}"/>
     <hyperlink ref="C2" r:id="rId15" xr:uid="{B49155BA-8B35-4CF5-A493-369B555F916E}"/>
     <hyperlink ref="C13" r:id="rId16" xr:uid="{381639CC-60AA-4F50-B17C-716C14BC8D31}"/>
-    <hyperlink ref="C22" r:id="rId17" xr:uid="{6F452CF8-3B37-4AE4-B788-3DED79D2AB45}"/>
-    <hyperlink ref="C18" r:id="rId18" xr:uid="{E769DE7B-FA73-4DEE-8BA9-CCEB20EB15B7}"/>
-    <hyperlink ref="C88" r:id="rId19" xr:uid="{6A51B699-F29C-4E09-899F-3B70831DE385}"/>
-    <hyperlink ref="C26" r:id="rId20" xr:uid="{4BED8ED8-6400-4F01-AC6A-64E3F7C4C068}"/>
-    <hyperlink ref="C93" r:id="rId21" xr:uid="{967B33AA-9669-432D-8143-542A4B48E69D}"/>
-    <hyperlink ref="C3" r:id="rId22" xr:uid="{3B8489A4-CB5E-4489-B2E9-CA4869059D30}"/>
-    <hyperlink ref="C92" r:id="rId23" xr:uid="{F4A51C44-639A-46C4-9693-1E59A9C5AAC4}"/>
-    <hyperlink ref="C12" r:id="rId24" xr:uid="{7886568F-C881-400E-B885-0068B0F42EFF}"/>
-    <hyperlink ref="C101" r:id="rId25" xr:uid="{A937FCBC-DB28-4CF7-94E2-6EFB29B8C7EC}"/>
-    <hyperlink ref="C25" r:id="rId26" xr:uid="{F1C45DAA-EE30-4045-AFDF-09AC63A9F22E}"/>
-    <hyperlink ref="C97" r:id="rId27" xr:uid="{DF692AF8-4315-4FEE-9E34-79929C30E712}"/>
-    <hyperlink ref="C91" r:id="rId28" xr:uid="{40C7E353-91FD-4E09-9086-CE268931F676}"/>
-    <hyperlink ref="C60" r:id="rId29" xr:uid="{E3A3CD2D-892D-4149-AA40-AE2D4608F772}"/>
-    <hyperlink ref="C76" r:id="rId30" xr:uid="{F670DB9B-E1EA-4B93-95BB-AEAD18258599}"/>
-    <hyperlink ref="C72" r:id="rId31" xr:uid="{78655D08-EB26-4D53-9E83-4C6559A0F853}"/>
-    <hyperlink ref="C35" r:id="rId32" xr:uid="{D94BCE83-ECC5-422C-8B9A-3CE0DE79C0E8}"/>
-    <hyperlink ref="C65" r:id="rId33" xr:uid="{B00893C1-292F-4DD5-A1A1-0FF6825C3326}"/>
-    <hyperlink ref="C49" r:id="rId34" xr:uid="{B16AF653-F238-404B-AB89-A4C838EE9D00}"/>
-    <hyperlink ref="C63" r:id="rId35" xr:uid="{F30EA5EF-A915-4FB0-85A3-FE240F62773D}"/>
-    <hyperlink ref="C74" r:id="rId36" xr:uid="{947C2B1A-0DC7-46BA-AF86-36B9FA37595F}"/>
-    <hyperlink ref="C57" r:id="rId37" xr:uid="{FB1164FE-9059-4AD8-ACEC-1DC322DC3889}"/>
-    <hyperlink ref="C75" r:id="rId38" xr:uid="{80E4A1DF-4D5A-41FC-BF2A-0EF156F339AF}"/>
-    <hyperlink ref="C85" r:id="rId39" xr:uid="{333B9245-C07B-4202-AEDF-5C2D04F18000}"/>
-    <hyperlink ref="C70" r:id="rId40" xr:uid="{0B5EB8E7-458D-4BDF-A1FD-77BAD567D698}"/>
-    <hyperlink ref="C59" r:id="rId41" xr:uid="{8C5D7768-B650-44E8-9273-C4EDE4849E6C}"/>
-    <hyperlink ref="C43" r:id="rId42" xr:uid="{12951A9E-F420-4509-A618-FF6E59020605}"/>
-    <hyperlink ref="C79" r:id="rId43" xr:uid="{CB72D7D2-2FAE-4804-B6E0-62722B216A28}"/>
-    <hyperlink ref="C48" r:id="rId44" xr:uid="{A6B098E7-DD37-4EF7-B910-FB1367C92999}"/>
-    <hyperlink ref="C66" r:id="rId45" xr:uid="{1CE9D879-CC7E-4C82-9E63-AFD8EB6D44ED}"/>
-    <hyperlink ref="C87" r:id="rId46" xr:uid="{7DEDCE9B-67FC-449F-8245-E5D46708FB94}"/>
-    <hyperlink ref="C32" r:id="rId47" xr:uid="{580F638E-B885-4B7F-A3D9-0ED70AFC642E}"/>
-    <hyperlink ref="C56" r:id="rId48" xr:uid="{9440C122-9053-445C-800A-F30D679D5119}"/>
-    <hyperlink ref="C67" r:id="rId49" xr:uid="{A58DB7B8-64E3-4436-B45D-6F6A6624DCDA}"/>
-    <hyperlink ref="C30" r:id="rId50" xr:uid="{F99D418D-2B38-48D9-B73E-3C0DFDA6D838}"/>
-    <hyperlink ref="C54" r:id="rId51" xr:uid="{A47ADE33-753F-4E2D-93DC-ECF2E05C0955}"/>
-    <hyperlink ref="C45" r:id="rId52" xr:uid="{B9CAC409-001C-4476-A51D-C47685E4D2D6}"/>
-    <hyperlink ref="C44" r:id="rId53" xr:uid="{665EB00F-B50E-4AAC-9D28-774ADADD3705}"/>
-    <hyperlink ref="C83" r:id="rId54" xr:uid="{FD2BD4A1-53D0-4536-98C9-F816B25A9496}"/>
-    <hyperlink ref="C71" r:id="rId55" xr:uid="{D4B9E531-1C99-49A5-AE65-A670DEB672D1}"/>
-    <hyperlink ref="C40" r:id="rId56" xr:uid="{6A223758-C219-4F20-A820-973A28F23CED}"/>
-    <hyperlink ref="C81" r:id="rId57" xr:uid="{32F5612D-0027-48FD-84C4-D22422144496}"/>
-    <hyperlink ref="C36" r:id="rId58" xr:uid="{E768C6BD-A2E2-4543-9B0A-DD78EE587E5B}"/>
-    <hyperlink ref="C69" r:id="rId59" xr:uid="{9386A92F-9D79-4C2A-AE88-C93CD0BB8EF3}"/>
-    <hyperlink ref="C55" r:id="rId60" xr:uid="{606EACAA-D502-411C-93EB-35E67B722CC3}"/>
-    <hyperlink ref="C68" r:id="rId61" xr:uid="{B39A4223-EBE3-4126-BE44-51B79639D0AB}"/>
-    <hyperlink ref="C51" r:id="rId62" xr:uid="{B42BC0F5-A385-4D2B-93FA-41A6674F4532}"/>
-    <hyperlink ref="C39" r:id="rId63" xr:uid="{5C34105E-87DC-420D-9049-087DDBF7B85A}"/>
-    <hyperlink ref="C38" r:id="rId64" xr:uid="{60FFB8B5-AB47-47F6-93A2-900E27C08FBC}"/>
-    <hyperlink ref="C62" r:id="rId65" xr:uid="{7A6835B4-3B41-4377-B6DA-16A57E750F63}"/>
-    <hyperlink ref="C61" r:id="rId66" xr:uid="{B9B8D59A-9F75-4F58-8372-35756F379A4F}"/>
-    <hyperlink ref="C33" r:id="rId67" xr:uid="{A8FE1516-4404-4D91-A367-BDFD828559AE}"/>
-    <hyperlink ref="C64" r:id="rId68" xr:uid="{A7346860-BC31-4AA9-ABD7-C84ABF4B6952}"/>
-    <hyperlink ref="C86" r:id="rId69" xr:uid="{395BE31C-6399-49F7-A2BC-105FAD65C472}"/>
-    <hyperlink ref="C52" r:id="rId70" xr:uid="{C09F011A-0B0E-40E2-99FE-7C2753733981}"/>
-    <hyperlink ref="C41" r:id="rId71" xr:uid="{26D5CA01-4CA7-4D5B-8DFE-ABA1D6D2C0CC}"/>
-    <hyperlink ref="C73" r:id="rId72" xr:uid="{4270B545-650C-42F5-BA98-B7561107846E}"/>
-    <hyperlink ref="C31" r:id="rId73" xr:uid="{BD922606-C8DA-4F21-A9A2-6626B70189D1}"/>
-    <hyperlink ref="C78" r:id="rId74" xr:uid="{A82A79E9-EF9E-4D70-AD41-B46E432A565C}"/>
-    <hyperlink ref="C53" r:id="rId75" xr:uid="{08AA4BDF-E5E6-4D5C-8BD0-D8E5C1872C8C}"/>
-    <hyperlink ref="C47" r:id="rId76" xr:uid="{C870E410-0B4F-4A29-B468-3CE8797E44B5}"/>
-    <hyperlink ref="C46" r:id="rId77" xr:uid="{E64F9C7F-A1B4-4494-917A-F4713B19D372}"/>
-    <hyperlink ref="C37" r:id="rId78" xr:uid="{D5D95D66-85D7-4303-9A29-76A48AD68844}"/>
-    <hyperlink ref="C29" r:id="rId79" xr:uid="{8A876D46-7765-4A59-B1C3-1D61B8E359A0}"/>
-    <hyperlink ref="C82" r:id="rId80" xr:uid="{852F532E-5370-47B6-BB7A-30BB2FAF2541}"/>
+    <hyperlink ref="C128" r:id="rId17" xr:uid="{6F452CF8-3B37-4AE4-B788-3DED79D2AB45}"/>
+    <hyperlink ref="C113" r:id="rId18" xr:uid="{6A51B699-F29C-4E09-899F-3B70831DE385}"/>
+    <hyperlink ref="C24" r:id="rId19" xr:uid="{4BED8ED8-6400-4F01-AC6A-64E3F7C4C068}"/>
+    <hyperlink ref="C118" r:id="rId20" xr:uid="{967B33AA-9669-432D-8143-542A4B48E69D}"/>
+    <hyperlink ref="C3" r:id="rId21" xr:uid="{3B8489A4-CB5E-4489-B2E9-CA4869059D30}"/>
+    <hyperlink ref="C117" r:id="rId22" xr:uid="{F4A51C44-639A-46C4-9693-1E59A9C5AAC4}"/>
+    <hyperlink ref="C12" r:id="rId23" xr:uid="{7886568F-C881-400E-B885-0068B0F42EFF}"/>
+    <hyperlink ref="C126" r:id="rId24" xr:uid="{A937FCBC-DB28-4CF7-94E2-6EFB29B8C7EC}"/>
+    <hyperlink ref="C23" r:id="rId25" xr:uid="{F1C45DAA-EE30-4045-AFDF-09AC63A9F22E}"/>
+    <hyperlink ref="C122" r:id="rId26" xr:uid="{DF692AF8-4315-4FEE-9E34-79929C30E712}"/>
+    <hyperlink ref="C116" r:id="rId27" xr:uid="{40C7E353-91FD-4E09-9086-CE268931F676}"/>
+    <hyperlink ref="C71" r:id="rId28" xr:uid="{E3A3CD2D-892D-4149-AA40-AE2D4608F772}"/>
+    <hyperlink ref="C89" r:id="rId29" xr:uid="{F670DB9B-E1EA-4B93-95BB-AEAD18258599}"/>
+    <hyperlink ref="C84" r:id="rId30" xr:uid="{78655D08-EB26-4D53-9E83-4C6559A0F853}"/>
+    <hyperlink ref="C35" r:id="rId31" xr:uid="{D94BCE83-ECC5-422C-8B9A-3CE0DE79C0E8}"/>
+    <hyperlink ref="C76" r:id="rId32" xr:uid="{B00893C1-292F-4DD5-A1A1-0FF6825C3326}"/>
+    <hyperlink ref="C57" r:id="rId33" xr:uid="{B16AF653-F238-404B-AB89-A4C838EE9D00}"/>
+    <hyperlink ref="C74" r:id="rId34" xr:uid="{F30EA5EF-A915-4FB0-85A3-FE240F62773D}"/>
+    <hyperlink ref="C86" r:id="rId35" xr:uid="{947C2B1A-0DC7-46BA-AF86-36B9FA37595F}"/>
+    <hyperlink ref="C68" r:id="rId36" xr:uid="{FB1164FE-9059-4AD8-ACEC-1DC322DC3889}"/>
+    <hyperlink ref="C87" r:id="rId37" xr:uid="{80E4A1DF-4D5A-41FC-BF2A-0EF156F339AF}"/>
+    <hyperlink ref="C107" r:id="rId38" xr:uid="{333B9245-C07B-4202-AEDF-5C2D04F18000}"/>
+    <hyperlink ref="C81" r:id="rId39" xr:uid="{0B5EB8E7-458D-4BDF-A1FD-77BAD567D698}"/>
+    <hyperlink ref="C70" r:id="rId40" xr:uid="{8C5D7768-B650-44E8-9273-C4EDE4849E6C}"/>
+    <hyperlink ref="C48" r:id="rId41" xr:uid="{12951A9E-F420-4509-A618-FF6E59020605}"/>
+    <hyperlink ref="C95" r:id="rId42" xr:uid="{CB72D7D2-2FAE-4804-B6E0-62722B216A28}"/>
+    <hyperlink ref="C56" r:id="rId43" xr:uid="{A6B098E7-DD37-4EF7-B910-FB1367C92999}"/>
+    <hyperlink ref="C77" r:id="rId44" xr:uid="{1CE9D879-CC7E-4C82-9E63-AFD8EB6D44ED}"/>
+    <hyperlink ref="C110" r:id="rId45" xr:uid="{7DEDCE9B-67FC-449F-8245-E5D46708FB94}"/>
+    <hyperlink ref="C32" r:id="rId46" xr:uid="{580F638E-B885-4B7F-A3D9-0ED70AFC642E}"/>
+    <hyperlink ref="C67" r:id="rId47" xr:uid="{9440C122-9053-445C-800A-F30D679D5119}"/>
+    <hyperlink ref="C78" r:id="rId48" xr:uid="{A58DB7B8-64E3-4436-B45D-6F6A6624DCDA}"/>
+    <hyperlink ref="C29" r:id="rId49" xr:uid="{F99D418D-2B38-48D9-B73E-3C0DFDA6D838}"/>
+    <hyperlink ref="C64" r:id="rId50" xr:uid="{A47ADE33-753F-4E2D-93DC-ECF2E05C0955}"/>
+    <hyperlink ref="C52" r:id="rId51" xr:uid="{B9CAC409-001C-4476-A51D-C47685E4D2D6}"/>
+    <hyperlink ref="C51" r:id="rId52" xr:uid="{665EB00F-B50E-4AAC-9D28-774ADADD3705}"/>
+    <hyperlink ref="C104" r:id="rId53" xr:uid="{FD2BD4A1-53D0-4536-98C9-F816B25A9496}"/>
+    <hyperlink ref="C82" r:id="rId54" xr:uid="{D4B9E531-1C99-49A5-AE65-A670DEB672D1}"/>
+    <hyperlink ref="C43" r:id="rId55" xr:uid="{6A223758-C219-4F20-A820-973A28F23CED}"/>
+    <hyperlink ref="C97" r:id="rId56" xr:uid="{32F5612D-0027-48FD-84C4-D22422144496}"/>
+    <hyperlink ref="C36" r:id="rId57" xr:uid="{E768C6BD-A2E2-4543-9B0A-DD78EE587E5B}"/>
+    <hyperlink ref="C80" r:id="rId58" xr:uid="{9386A92F-9D79-4C2A-AE88-C93CD0BB8EF3}"/>
+    <hyperlink ref="C66" r:id="rId59" xr:uid="{606EACAA-D502-411C-93EB-35E67B722CC3}"/>
+    <hyperlink ref="C79" r:id="rId60" xr:uid="{B39A4223-EBE3-4126-BE44-51B79639D0AB}"/>
+    <hyperlink ref="C61" r:id="rId61" xr:uid="{B42BC0F5-A385-4D2B-93FA-41A6674F4532}"/>
+    <hyperlink ref="C39" r:id="rId62" xr:uid="{5C34105E-87DC-420D-9049-087DDBF7B85A}"/>
+    <hyperlink ref="C38" r:id="rId63" xr:uid="{60FFB8B5-AB47-47F6-93A2-900E27C08FBC}"/>
+    <hyperlink ref="C73" r:id="rId64" xr:uid="{7A6835B4-3B41-4377-B6DA-16A57E750F63}"/>
+    <hyperlink ref="C72" r:id="rId65" xr:uid="{B9B8D59A-9F75-4F58-8372-35756F379A4F}"/>
+    <hyperlink ref="C33" r:id="rId66" xr:uid="{A8FE1516-4404-4D91-A367-BDFD828559AE}"/>
+    <hyperlink ref="C75" r:id="rId67" xr:uid="{A7346860-BC31-4AA9-ABD7-C84ABF4B6952}"/>
+    <hyperlink ref="C109" r:id="rId68" xr:uid="{395BE31C-6399-49F7-A2BC-105FAD65C472}"/>
+    <hyperlink ref="C62" r:id="rId69" xr:uid="{C09F011A-0B0E-40E2-99FE-7C2753733981}"/>
+    <hyperlink ref="C45" r:id="rId70" xr:uid="{26D5CA01-4CA7-4D5B-8DFE-ABA1D6D2C0CC}"/>
+    <hyperlink ref="C85" r:id="rId71" xr:uid="{4270B545-650C-42F5-BA98-B7561107846E}"/>
+    <hyperlink ref="C31" r:id="rId72" xr:uid="{BD922606-C8DA-4F21-A9A2-6626B70189D1}"/>
+    <hyperlink ref="C94" r:id="rId73" xr:uid="{A82A79E9-EF9E-4D70-AD41-B46E432A565C}"/>
+    <hyperlink ref="C63" r:id="rId74" xr:uid="{08AA4BDF-E5E6-4D5C-8BD0-D8E5C1872C8C}"/>
+    <hyperlink ref="C55" r:id="rId75" xr:uid="{C870E410-0B4F-4A29-B468-3CE8797E44B5}"/>
+    <hyperlink ref="C53" r:id="rId76" xr:uid="{E64F9C7F-A1B4-4494-917A-F4713B19D372}"/>
+    <hyperlink ref="C37" r:id="rId77" xr:uid="{D5D95D66-85D7-4303-9A29-76A48AD68844}"/>
+    <hyperlink ref="C28" r:id="rId78" xr:uid="{8A876D46-7765-4A59-B1C3-1D61B8E359A0}"/>
+    <hyperlink ref="C100" r:id="rId79" xr:uid="{852F532E-5370-47B6-BB7A-30BB2FAF2541}"/>
+    <hyperlink ref="C91" r:id="rId80" xr:uid="{186BECEB-1495-4ECF-A87F-077CB400C8A8}"/>
+    <hyperlink ref="C103" r:id="rId81" xr:uid="{756BB6A1-2261-4569-A4DF-AAFB369C40F4}"/>
+    <hyperlink ref="C127" r:id="rId82" xr:uid="{E769DE7B-FA73-4DEE-8BA9-CCEB20EB15B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId81"/>
+  <pageSetup orientation="portrait" r:id="rId83"/>
 </worksheet>
 </file>
 
@@ -8136,7 +8623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABB5F57-9A03-4145-8201-5FC47AB315FD}">
   <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+    <sheetView topLeftCell="A124" workbookViewId="0">
       <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>

</xml_diff>